<commit_message>
Published state of ETDataset on 23 August 2016
</commit_message>
<xml_diff>
--- a/analyses/4b_chemical_industry_analysis.xlsx
+++ b/analyses/4b_chemical_industry_analysis.xlsx
@@ -18264,7 +18264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" outlineLevel="1">
+    <row r="39" spans="1:16" hidden="1" outlineLevel="1">
       <c r="A39" s="8"/>
       <c r="B39" s="31"/>
       <c r="C39" s="257"/>
@@ -18282,7 +18282,7 @@
       <c r="O39" s="207"/>
       <c r="P39" s="208"/>
     </row>
-    <row r="40" spans="1:16" outlineLevel="1">
+    <row r="40" spans="1:16" hidden="1" outlineLevel="1">
       <c r="A40" s="8"/>
       <c r="B40" s="28" t="s">
         <v>310</v>
@@ -18302,7 +18302,7 @@
       <c r="O40" s="207"/>
       <c r="P40" s="208"/>
     </row>
-    <row r="41" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="41" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A41" s="8"/>
       <c r="B41" s="22" t="s">
         <v>283</v>
@@ -18322,7 +18322,7 @@
       <c r="O41" s="207"/>
       <c r="P41" s="208"/>
     </row>
-    <row r="42" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="42" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A42" s="8"/>
       <c r="B42" s="22"/>
       <c r="C42" s="258" t="s">
@@ -18331,7 +18331,10 @@
       <c r="D42" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E42" s="291"/>
+      <c r="E42" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F42" s="126"/>
       <c r="G42" s="202"/>
       <c r="H42" s="8"/>
@@ -18342,7 +18345,7 @@
       </c>
       <c r="L42" s="242" t="b">
         <f>IF((E42)&lt;='Fuel aggregation'!E15, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" s="280"/>
       <c r="N42" s="8"/>
@@ -18351,10 +18354,10 @@
       </c>
       <c r="P42" s="7">
         <f t="shared" ref="P42:P47" si="0">IF(L42=TRUE,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A43" s="8"/>
       <c r="B43" s="22"/>
       <c r="C43" s="258" t="s">
@@ -18363,7 +18366,10 @@
       <c r="D43" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E43" s="291"/>
+      <c r="E43" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F43" s="126"/>
       <c r="G43" s="202"/>
       <c r="H43" s="8"/>
@@ -18374,7 +18380,7 @@
       </c>
       <c r="L43" s="242" t="b">
         <f>IF((E43)&lt;='Fuel aggregation'!H15, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M43" s="280"/>
       <c r="N43" s="8"/>
@@ -18383,10 +18389,10 @@
       </c>
       <c r="P43" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A44" s="8"/>
       <c r="B44" s="22"/>
       <c r="C44" s="258" t="s">
@@ -18395,7 +18401,10 @@
       <c r="D44" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E44" s="291"/>
+      <c r="E44" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F44" s="126"/>
       <c r="G44" s="202"/>
       <c r="H44" s="8"/>
@@ -18406,7 +18415,7 @@
       </c>
       <c r="L44" s="242" t="b">
         <f>IF((E44)&lt;='Fuel aggregation'!I15, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44" s="280"/>
       <c r="N44" s="8"/>
@@ -18415,10 +18424,10 @@
       </c>
       <c r="P44" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A45" s="8"/>
       <c r="B45" s="22"/>
       <c r="C45" s="258" t="s">
@@ -18427,7 +18436,10 @@
       <c r="D45" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E45" s="291"/>
+      <c r="E45" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F45" s="126"/>
       <c r="G45" s="202"/>
       <c r="H45" s="8"/>
@@ -18438,7 +18450,7 @@
       </c>
       <c r="L45" s="242" t="b">
         <f>IF((E45)&lt;='Fuel aggregation'!J15, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="280"/>
       <c r="N45" s="8"/>
@@ -18447,10 +18459,10 @@
       </c>
       <c r="P45" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A46" s="8"/>
       <c r="B46" s="22"/>
       <c r="C46" s="258" t="s">
@@ -18459,7 +18471,10 @@
       <c r="D46" s="292" t="s">
         <v>225</v>
       </c>
-      <c r="E46" s="291"/>
+      <c r="E46" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F46" s="126"/>
       <c r="G46" s="202"/>
       <c r="H46" s="8"/>
@@ -18470,7 +18485,7 @@
       </c>
       <c r="L46" s="242" t="b">
         <f>IF((E46)&lt;='Fuel aggregation'!K15, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M46" s="280"/>
       <c r="N46" s="8"/>
@@ -18479,10 +18494,10 @@
       </c>
       <c r="P46" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A47" s="8"/>
       <c r="B47" s="22"/>
       <c r="C47" s="258" t="s">
@@ -18491,7 +18506,10 @@
       <c r="D47" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E47" s="291"/>
+      <c r="E47" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F47" s="126"/>
       <c r="G47" s="202"/>
       <c r="H47" s="8"/>
@@ -18502,7 +18520,7 @@
       </c>
       <c r="L47" s="242" t="b">
         <f>IF((E47)&lt;='Fuel aggregation'!L15, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M47" s="280"/>
       <c r="N47" s="8"/>
@@ -18511,10 +18529,10 @@
       </c>
       <c r="P47" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" outlineLevel="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" hidden="1" outlineLevel="1">
       <c r="A48" s="8"/>
       <c r="B48" s="22"/>
       <c r="C48" s="202"/>
@@ -18532,7 +18550,7 @@
       <c r="O48" s="207"/>
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="49" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A49" s="8"/>
       <c r="B49" s="22" t="s">
         <v>284</v>
@@ -18552,7 +18570,7 @@
       <c r="O49" s="207"/>
       <c r="P49" s="208"/>
     </row>
-    <row r="50" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A50" s="8"/>
       <c r="B50" s="22"/>
       <c r="C50" s="258" t="s">
@@ -18561,7 +18579,10 @@
       <c r="D50" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E50" s="291"/>
+      <c r="E50" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F50" s="126"/>
       <c r="G50" s="202"/>
       <c r="H50" s="8"/>
@@ -18572,7 +18593,7 @@
       </c>
       <c r="L50" s="242" t="b">
         <f>IF((E50)&lt;='Fuel aggregation'!E22, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M50" s="280"/>
       <c r="N50" s="8"/>
@@ -18581,10 +18602,10 @@
       </c>
       <c r="P50" s="7">
         <f t="shared" ref="P50:P52" si="1">IF(L50=TRUE,1,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A51" s="8"/>
       <c r="B51" s="22"/>
       <c r="C51" s="258" t="s">
@@ -18593,7 +18614,10 @@
       <c r="D51" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E51" s="291"/>
+      <c r="E51" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F51" s="126"/>
       <c r="G51" s="202"/>
       <c r="H51" s="8"/>
@@ -18604,7 +18628,7 @@
       </c>
       <c r="L51" s="242" t="b">
         <f>IF((E51)&lt;='Fuel aggregation'!H22, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M51" s="280"/>
       <c r="N51" s="8"/>
@@ -18613,10 +18637,10 @@
       </c>
       <c r="P51" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
       <c r="A52" s="8"/>
       <c r="B52" s="22"/>
       <c r="C52" s="258" t="s">
@@ -18625,7 +18649,10 @@
       <c r="D52" s="158" t="s">
         <v>225</v>
       </c>
-      <c r="E52" s="291"/>
+      <c r="E52" s="291" t="str">
+        <f>IF(E38="no",0,"")</f>
+        <v/>
+      </c>
       <c r="F52" s="126"/>
       <c r="G52" s="202"/>
       <c r="H52" s="8"/>
@@ -18636,7 +18663,7 @@
       </c>
       <c r="L52" s="242" t="b">
         <f>IF(E52&lt;='Fuel aggregation'!I22, TRUE, FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M52" s="280"/>
       <c r="N52" s="8"/>
@@ -18645,10 +18672,10 @@
       </c>
       <c r="P52" s="7">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" ht="16" thickBot="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="16" collapsed="1" thickBot="1">
       <c r="B53" s="33"/>
       <c r="C53" s="46"/>
       <c r="D53" s="159"/>

</xml_diff>

<commit_message>
Published state of ETDataset on 2 September 2016
</commit_message>
<xml_diff>
--- a/analyses/4b_chemical_industry_analysis.xlsx
+++ b/analyses/4b_chemical_industry_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27322"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16100" tabRatio="835" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23520" tabRatio="835" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -23,39 +23,43 @@
     <sheet name="Refineries transformation" sheetId="109" r:id="rId14"/>
     <sheet name="Refineries heat production" sheetId="111" r:id="rId15"/>
     <sheet name="Refineries efficiency" sheetId="112" r:id="rId16"/>
-    <sheet name="csv_export_to_industry_analysis" sheetId="96" r:id="rId17"/>
-    <sheet name="csv_chemical_coal_e_ps" sheetId="97" r:id="rId18"/>
-    <sheet name="csv_chemical_network_gas_e_ps" sheetId="100" r:id="rId19"/>
-    <sheet name="csv_chemical_crude_oil_e_ps" sheetId="101" r:id="rId20"/>
-    <sheet name="csv_chemical_wood_pellets_e_ps" sheetId="102" r:id="rId21"/>
-    <sheet name="csv_chemical_steam_hot_water_ps" sheetId="103" r:id="rId22"/>
-    <sheet name="csv_chemical_electricity_ps" sheetId="104" r:id="rId23"/>
-    <sheet name="csv_chemical_coal_non_e_ps" sheetId="105" r:id="rId24"/>
-    <sheet name="csv_chemical_gas_non_e_ps" sheetId="106" r:id="rId25"/>
-    <sheet name="csv_chemical_crude_oil_non_e_ps" sheetId="107" r:id="rId26"/>
-    <sheet name="csv_chemical_wood_non_e_ps" sheetId="108" r:id="rId27"/>
-    <sheet name="csv_refinery_transformation_eff" sheetId="110" r:id="rId28"/>
+    <sheet name="Steam methane reformer input" sheetId="113" r:id="rId17"/>
+    <sheet name="csv_export_to_industry_analysis" sheetId="96" r:id="rId18"/>
+    <sheet name="csv_chemical_coal_e_ps" sheetId="97" r:id="rId19"/>
+    <sheet name="csv_chemical_network_gas_e_ps" sheetId="100" r:id="rId20"/>
+    <sheet name="csv_chemical_crude_oil_e_ps" sheetId="101" r:id="rId21"/>
+    <sheet name="csv_chemical_wood_pellets_e_ps" sheetId="102" r:id="rId22"/>
+    <sheet name="csv_chemical_steam_hot_water_ps" sheetId="103" r:id="rId23"/>
+    <sheet name="csv_chemical_electricity_ps" sheetId="104" r:id="rId24"/>
+    <sheet name="csv_chemical_coal_non_e_ps" sheetId="105" r:id="rId25"/>
+    <sheet name="csv_chemical_gas_non_e_ps" sheetId="106" r:id="rId26"/>
+    <sheet name="csv_chemical_crude_oil_non_e_ps" sheetId="107" r:id="rId27"/>
+    <sheet name="csv_chemical_wood_non_e_ps" sheetId="108" r:id="rId28"/>
+    <sheet name="csv_refinery_transformation_eff" sheetId="110" r:id="rId29"/>
+    <sheet name="csv_steam_methane_reformer_eff" sheetId="114" r:id="rId30"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId29"/>
+    <externalReference r:id="rId31"/>
   </externalReferences>
   <definedNames>
-    <definedName name="aluminium_production" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="aluminium_production" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="aluminium_production" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="aluminium_production" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="aluminium_production" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="aluminium_production" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="aluminium_production" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="aluminium_production" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="aluminium_production">Dashboard!#REF!</definedName>
     <definedName name="base_year">Dashboard!$E$14</definedName>
     <definedName name="country">Dashboard!$E$13</definedName>
@@ -65,12 +69,14 @@
     <definedName name="Eff_Airco" localSheetId="13">'[1]Technological specifications'!$F$25</definedName>
     <definedName name="Eff_Airco" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Airco" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Airco" localSheetId="16">'[1]Technological specifications'!$F$25</definedName>
     <definedName name="Eff_Biomass_Heater" localSheetId="12">'[1]Technological specifications'!$F$19</definedName>
     <definedName name="Eff_Biomass_Heater" localSheetId="15">'[1]Technological specifications'!$F$19</definedName>
     <definedName name="Eff_Biomass_Heater" localSheetId="14">'[1]Technological specifications'!$F$19</definedName>
     <definedName name="Eff_Biomass_Heater" localSheetId="13">'[1]Technological specifications'!$F$19</definedName>
     <definedName name="Eff_Biomass_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Biomass_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Biomass_Heater" localSheetId="16">'[1]Technological specifications'!$F$19</definedName>
     <definedName name="Eff_Centralized_Heater" localSheetId="4">#REF!</definedName>
     <definedName name="Eff_Centralized_Heater" localSheetId="12">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Eff_Centralized_Heater" localSheetId="15">'[1]Technological specifications'!#REF!</definedName>
@@ -78,66 +84,77 @@
     <definedName name="Eff_Centralized_Heater" localSheetId="13">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Eff_Centralized_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Centralized_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Centralized_Heater" localSheetId="16">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Eff_Coal_Heater" localSheetId="12">'[1]Technological specifications'!$F$17</definedName>
     <definedName name="Eff_Coal_Heater" localSheetId="15">'[1]Technological specifications'!$F$17</definedName>
     <definedName name="Eff_Coal_Heater" localSheetId="14">'[1]Technological specifications'!$F$17</definedName>
     <definedName name="Eff_Coal_Heater" localSheetId="13">'[1]Technological specifications'!$F$17</definedName>
     <definedName name="Eff_Coal_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Coal_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Coal_Heater" localSheetId="16">'[1]Technological specifications'!$F$17</definedName>
     <definedName name="Eff_Distr_Heater" localSheetId="12">'[1]Technological specifications'!$F$20</definedName>
     <definedName name="Eff_Distr_Heater" localSheetId="15">'[1]Technological specifications'!$F$20</definedName>
     <definedName name="Eff_Distr_Heater" localSheetId="14">'[1]Technological specifications'!$F$20</definedName>
     <definedName name="Eff_Distr_Heater" localSheetId="13">'[1]Technological specifications'!$F$20</definedName>
     <definedName name="Eff_Distr_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Distr_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Distr_Heater" localSheetId="16">'[1]Technological specifications'!$F$20</definedName>
     <definedName name="Eff_Elec_Cold_Pump" localSheetId="12">'[1]Technological specifications'!$F$24</definedName>
     <definedName name="Eff_Elec_Cold_Pump" localSheetId="15">'[1]Technological specifications'!$F$24</definedName>
     <definedName name="Eff_Elec_Cold_Pump" localSheetId="14">'[1]Technological specifications'!$F$24</definedName>
     <definedName name="Eff_Elec_Cold_Pump" localSheetId="13">'[1]Technological specifications'!$F$24</definedName>
     <definedName name="Eff_Elec_Cold_Pump" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Elec_Cold_Pump" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Elec_Cold_Pump" localSheetId="16">'[1]Technological specifications'!$F$24</definedName>
     <definedName name="Eff_Elec_Heat_Pump" localSheetId="12">'[1]Technological specifications'!$F$14</definedName>
     <definedName name="Eff_Elec_Heat_Pump" localSheetId="15">'[1]Technological specifications'!$F$14</definedName>
     <definedName name="Eff_Elec_Heat_Pump" localSheetId="14">'[1]Technological specifications'!$F$14</definedName>
     <definedName name="Eff_Elec_Heat_Pump" localSheetId="13">'[1]Technological specifications'!$F$14</definedName>
     <definedName name="Eff_Elec_Heat_Pump" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Elec_Heat_Pump" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Elec_Heat_Pump" localSheetId="16">'[1]Technological specifications'!$F$14</definedName>
     <definedName name="Eff_Elec_Heater" localSheetId="12">'[1]Technological specifications'!$F$15</definedName>
     <definedName name="Eff_Elec_Heater" localSheetId="15">'[1]Technological specifications'!$F$15</definedName>
     <definedName name="Eff_Elec_Heater" localSheetId="14">'[1]Technological specifications'!$F$15</definedName>
     <definedName name="Eff_Elec_Heater" localSheetId="13">'[1]Technological specifications'!$F$15</definedName>
     <definedName name="Eff_Elec_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Elec_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Elec_Heater" localSheetId="16">'[1]Technological specifications'!$F$15</definedName>
     <definedName name="Eff_Fluo_Lamp" localSheetId="12">'[1]Technological specifications'!$F$29</definedName>
     <definedName name="Eff_Fluo_Lamp" localSheetId="15">'[1]Technological specifications'!$F$29</definedName>
     <definedName name="Eff_Fluo_Lamp" localSheetId="14">'[1]Technological specifications'!$F$29</definedName>
     <definedName name="Eff_Fluo_Lamp" localSheetId="13">'[1]Technological specifications'!$F$29</definedName>
     <definedName name="Eff_Fluo_Lamp" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Fluo_Lamp" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Fluo_Lamp" localSheetId="16">'[1]Technological specifications'!$F$29</definedName>
     <definedName name="Eff_Fluo_Tube" localSheetId="12">'[1]Technological specifications'!$F$30</definedName>
     <definedName name="Eff_Fluo_Tube" localSheetId="15">'[1]Technological specifications'!$F$30</definedName>
     <definedName name="Eff_Fluo_Tube" localSheetId="14">'[1]Technological specifications'!$F$30</definedName>
     <definedName name="Eff_Fluo_Tube" localSheetId="13">'[1]Technological specifications'!$F$30</definedName>
     <definedName name="Eff_Fluo_Tube" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Fluo_Tube" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Fluo_Tube" localSheetId="16">'[1]Technological specifications'!$F$30</definedName>
     <definedName name="Eff_Gas_Cold_Pump" localSheetId="12">'[1]Technological specifications'!$F$23</definedName>
     <definedName name="Eff_Gas_Cold_Pump" localSheetId="15">'[1]Technological specifications'!$F$23</definedName>
     <definedName name="Eff_Gas_Cold_Pump" localSheetId="14">'[1]Technological specifications'!$F$23</definedName>
     <definedName name="Eff_Gas_Cold_Pump" localSheetId="13">'[1]Technological specifications'!$F$23</definedName>
     <definedName name="Eff_Gas_Cold_Pump" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Gas_Cold_Pump" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Gas_Cold_Pump" localSheetId="16">'[1]Technological specifications'!$F$23</definedName>
     <definedName name="Eff_Gas_Heat_Pump" localSheetId="12">'[1]Technological specifications'!$F$13</definedName>
     <definedName name="Eff_Gas_Heat_Pump" localSheetId="15">'[1]Technological specifications'!$F$13</definedName>
     <definedName name="Eff_Gas_Heat_Pump" localSheetId="14">'[1]Technological specifications'!$F$13</definedName>
     <definedName name="Eff_Gas_Heat_Pump" localSheetId="13">'[1]Technological specifications'!$F$13</definedName>
     <definedName name="Eff_Gas_Heat_Pump" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Gas_Heat_Pump" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Gas_Heat_Pump" localSheetId="16">'[1]Technological specifications'!$F$13</definedName>
     <definedName name="Eff_Gas_Heater" localSheetId="12">'[1]Technological specifications'!$F$12</definedName>
     <definedName name="Eff_Gas_Heater" localSheetId="15">'[1]Technological specifications'!$F$12</definedName>
     <definedName name="Eff_Gas_Heater" localSheetId="14">'[1]Technological specifications'!$F$12</definedName>
     <definedName name="Eff_Gas_Heater" localSheetId="13">'[1]Technological specifications'!$F$12</definedName>
     <definedName name="Eff_Gas_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Gas_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Gas_Heater" localSheetId="16">'[1]Technological specifications'!$F$12</definedName>
     <definedName name="Eff_Gas_Heater">'Final demand'!$E$11</definedName>
     <definedName name="Eff_Geothermal_Heater" localSheetId="4">#REF!</definedName>
     <definedName name="Eff_Geothermal_Heater" localSheetId="12">'[1]Technological specifications'!#REF!</definedName>
@@ -146,54 +163,65 @@
     <definedName name="Eff_Geothermal_Heater" localSheetId="13">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Eff_Geothermal_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Geothermal_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Geothermal_Heater" localSheetId="16">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Eff_Incan_Lamp" localSheetId="12">'[1]Technological specifications'!$F$28</definedName>
     <definedName name="Eff_Incan_Lamp" localSheetId="15">'[1]Technological specifications'!$F$28</definedName>
     <definedName name="Eff_Incan_Lamp" localSheetId="14">'[1]Technological specifications'!$F$28</definedName>
     <definedName name="Eff_Incan_Lamp" localSheetId="13">'[1]Technological specifications'!$F$28</definedName>
     <definedName name="Eff_Incan_Lamp" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Incan_Lamp" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Incan_Lamp" localSheetId="16">'[1]Technological specifications'!$F$28</definedName>
     <definedName name="Eff_LED_Lamp" localSheetId="12">'[1]Technological specifications'!$F$31</definedName>
     <definedName name="Eff_LED_Lamp" localSheetId="15">'[1]Technological specifications'!$F$31</definedName>
     <definedName name="Eff_LED_Lamp" localSheetId="14">'[1]Technological specifications'!$F$31</definedName>
     <definedName name="Eff_LED_Lamp" localSheetId="13">'[1]Technological specifications'!$F$31</definedName>
     <definedName name="Eff_LED_Lamp" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_LED_Lamp" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_LED_Lamp" localSheetId="16">'[1]Technological specifications'!$F$31</definedName>
     <definedName name="Eff_Oil_Heater" localSheetId="12">'[1]Technological specifications'!$F$18</definedName>
     <definedName name="Eff_Oil_Heater" localSheetId="15">'[1]Technological specifications'!$F$18</definedName>
     <definedName name="Eff_Oil_Heater" localSheetId="14">'[1]Technological specifications'!$F$18</definedName>
     <definedName name="Eff_Oil_Heater" localSheetId="13">'[1]Technological specifications'!$F$18</definedName>
     <definedName name="Eff_Oil_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Oil_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Oil_Heater" localSheetId="16">'[1]Technological specifications'!$F$18</definedName>
     <definedName name="Eff_Solar_Heater" localSheetId="12">'[1]Technological specifications'!$F$16</definedName>
     <definedName name="Eff_Solar_Heater" localSheetId="15">'[1]Technological specifications'!$F$16</definedName>
     <definedName name="Eff_Solar_Heater" localSheetId="14">'[1]Technological specifications'!$F$16</definedName>
     <definedName name="Eff_Solar_Heater" localSheetId="13">'[1]Technological specifications'!$F$16</definedName>
     <definedName name="Eff_Solar_Heater" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Eff_Solar_Heater" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Eff_Solar_Heater" localSheetId="16">'[1]Technological specifications'!$F$16</definedName>
     <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="12">'[1]Corrected energy balance'!$BN$84</definedName>
     <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="15">'[1]Corrected energy balance'!$BN$84</definedName>
     <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="14">'[1]Corrected energy balance'!$BN$84</definedName>
     <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="13">'[1]Corrected energy balance'!$BN$84</definedName>
+    <definedName name="Final_Demand_Comm_and_Publ_Services" localSheetId="16">'[1]Corrected energy balance'!$BN$84</definedName>
     <definedName name="Final_Demand_Electrical_Appliances" localSheetId="12">'[1]Final demand per energy carrier'!$F$41</definedName>
     <definedName name="Final_Demand_Electrical_Appliances" localSheetId="15">'[1]Final demand per energy carrier'!$F$41</definedName>
     <definedName name="Final_Demand_Electrical_Appliances" localSheetId="14">'[1]Final demand per energy carrier'!$F$41</definedName>
     <definedName name="Final_Demand_Electrical_Appliances" localSheetId="13">'[1]Final demand per energy carrier'!$F$41</definedName>
+    <definedName name="Final_Demand_Electrical_Appliances" localSheetId="16">'[1]Final demand per energy carrier'!$F$41</definedName>
     <definedName name="Final_Demand_Lighting" localSheetId="12">[1]Dashboard!$D$26</definedName>
     <definedName name="Final_Demand_Lighting" localSheetId="15">[1]Dashboard!$D$26</definedName>
     <definedName name="Final_Demand_Lighting" localSheetId="14">[1]Dashboard!$D$26</definedName>
     <definedName name="Final_Demand_Lighting" localSheetId="13">[1]Dashboard!$D$26</definedName>
+    <definedName name="Final_Demand_Lighting" localSheetId="16">[1]Dashboard!$D$26</definedName>
     <definedName name="Final_Demand_Other_Appliances" localSheetId="12">[1]Dashboard!$D$29</definedName>
     <definedName name="Final_Demand_Other_Appliances" localSheetId="15">[1]Dashboard!$D$29</definedName>
     <definedName name="Final_Demand_Other_Appliances" localSheetId="14">[1]Dashboard!$D$29</definedName>
     <definedName name="Final_Demand_Other_Appliances" localSheetId="13">[1]Dashboard!$D$29</definedName>
+    <definedName name="Final_Demand_Other_Appliances" localSheetId="16">[1]Dashboard!$D$29</definedName>
     <definedName name="Final_Demand_Space_Cooling" localSheetId="12">[1]Dashboard!$D$25</definedName>
     <definedName name="Final_Demand_Space_Cooling" localSheetId="15">[1]Dashboard!$D$25</definedName>
     <definedName name="Final_Demand_Space_Cooling" localSheetId="14">[1]Dashboard!$D$25</definedName>
     <definedName name="Final_Demand_Space_Cooling" localSheetId="13">[1]Dashboard!$D$25</definedName>
+    <definedName name="Final_Demand_Space_Cooling" localSheetId="16">[1]Dashboard!$D$25</definedName>
     <definedName name="Final_demand_Space_Heating" localSheetId="12">[1]Dashboard!$D$24</definedName>
     <definedName name="Final_demand_Space_Heating" localSheetId="15">[1]Dashboard!$D$24</definedName>
     <definedName name="Final_demand_Space_Heating" localSheetId="14">[1]Dashboard!$D$24</definedName>
     <definedName name="Final_demand_Space_Heating" localSheetId="13">[1]Dashboard!$D$24</definedName>
+    <definedName name="Final_demand_Space_Heating" localSheetId="16">[1]Dashboard!$D$24</definedName>
     <definedName name="GWh_to_TJ" localSheetId="9">[1]Assumptions!$C$131</definedName>
     <definedName name="GWh_to_TJ" localSheetId="12">[1]Assumptions!$C$131</definedName>
     <definedName name="GWh_to_TJ" localSheetId="15">[1]Assumptions!$C$131</definedName>
@@ -201,6 +229,7 @@
     <definedName name="GWh_to_TJ" localSheetId="13">[1]Assumptions!$C$131</definedName>
     <definedName name="GWh_to_TJ" localSheetId="10">[1]Assumptions!$C$131</definedName>
     <definedName name="GWh_to_TJ" localSheetId="11">[1]Assumptions!$C$131</definedName>
+    <definedName name="GWh_to_TJ" localSheetId="16">[1]Assumptions!$C$131</definedName>
     <definedName name="GWh_to_TJ" localSheetId="8">[1]Assumptions!$C$131</definedName>
     <definedName name="Heat_eff_Biogas_CHP" localSheetId="4">#REF!</definedName>
     <definedName name="Heat_eff_Biogas_CHP" localSheetId="12">'[1]Technological specifications'!#REF!</definedName>
@@ -209,6 +238,7 @@
     <definedName name="Heat_eff_Biogas_CHP" localSheetId="13">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Heat_eff_Biogas_CHP" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Heat_eff_Biogas_CHP" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Heat_eff_Biogas_CHP" localSheetId="16">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Heat_Eff_Biomass_CHP" localSheetId="4">#REF!</definedName>
     <definedName name="Heat_Eff_Biomass_CHP" localSheetId="9">'Final demand'!#REF!</definedName>
     <definedName name="Heat_Eff_Biomass_CHP" localSheetId="12">'[1]Technological specifications'!#REF!</definedName>
@@ -217,6 +247,7 @@
     <definedName name="Heat_Eff_Biomass_CHP" localSheetId="13">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Heat_Eff_Biomass_CHP" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Heat_Eff_Biomass_CHP" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Heat_Eff_Biomass_CHP" localSheetId="16">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Heat_Eff_Gas_CHP" localSheetId="4">#REF!</definedName>
     <definedName name="Heat_Eff_Gas_CHP" localSheetId="9">'Final demand'!#REF!</definedName>
     <definedName name="Heat_Eff_Gas_CHP" localSheetId="12">'[1]Technological specifications'!#REF!</definedName>
@@ -225,308 +256,362 @@
     <definedName name="Heat_Eff_Gas_CHP" localSheetId="13">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Heat_Eff_Gas_CHP" localSheetId="10">'Shares energetic final demand'!#REF!</definedName>
     <definedName name="Heat_Eff_Gas_CHP" localSheetId="11">'Shares non-energ final demand'!#REF!</definedName>
+    <definedName name="Heat_Eff_Gas_CHP" localSheetId="16">'[1]Technological specifications'!#REF!</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="12">'[1]Technology split of final deman'!$G$31</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="15">'[1]Technology split of final deman'!$G$31</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="14">'[1]Technology split of final deman'!$G$31</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="13">'[1]Technology split of final deman'!$G$31</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_Fluo_Lamps" localSheetId="16">'[1]Technology split of final deman'!$G$31</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="12">'[1]Technology split of final deman'!$G$32</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="15">'[1]Technology split of final deman'!$G$32</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="14">'[1]Technology split of final deman'!$G$32</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="13">'[1]Technology split of final deman'!$G$32</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_Fluo_Tubes" localSheetId="16">'[1]Technology split of final deman'!$G$32</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="12">'[1]Technology split of final deman'!$G$30</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="15">'[1]Technology split of final deman'!$G$30</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="14">'[1]Technology split of final deman'!$G$30</definedName>
     <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="13">'[1]Technology split of final deman'!$G$30</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_Incan_Lamps" localSheetId="16">'[1]Technology split of final deman'!$G$30</definedName>
     <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="12">'[1]Technology split of final deman'!$G$33</definedName>
     <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="15">'[1]Technology split of final deman'!$G$33</definedName>
     <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="14">'[1]Technology split of final deman'!$G$33</definedName>
     <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="13">'[1]Technology split of final deman'!$G$33</definedName>
+    <definedName name="Perc_Final_Demand_Lighting_LED_Lamps" localSheetId="16">'[1]Technology split of final deman'!$G$33</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="12">'[1]Technology split of final deman'!$G$25</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="15">'[1]Technology split of final deman'!$G$25</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="14">'[1]Technology split of final deman'!$G$25</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="13">'[1]Technology split of final deman'!$G$25</definedName>
+    <definedName name="Perc_Final_Demand_Space_Cooling_Airco" localSheetId="16">'[1]Technology split of final deman'!$G$25</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="12">'[1]Technology split of final deman'!$G$24</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="15">'[1]Technology split of final deman'!$G$24</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="14">'[1]Technology split of final deman'!$G$24</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="13">'[1]Technology split of final deman'!$G$24</definedName>
+    <definedName name="Perc_Final_Demand_Space_Cooling_Elec_Heat_Pump" localSheetId="16">'[1]Technology split of final deman'!$G$24</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="12">'[1]Technology split of final deman'!$G$23</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="15">'[1]Technology split of final deman'!$G$23</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="14">'[1]Technology split of final deman'!$G$23</definedName>
     <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="13">'[1]Technology split of final deman'!$G$23</definedName>
+    <definedName name="Perc_Final_Demand_Space_Cooling_Gas_Heat_Pump" localSheetId="16">'[1]Technology split of final deman'!$G$23</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="12">'[1]Technology split of final deman'!$G$17</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="15">'[1]Technology split of final deman'!$G$17</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="14">'[1]Technology split of final deman'!$G$17</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="13">'[1]Technology split of final deman'!$G$17</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Biomass_Heater" localSheetId="16">'[1]Technology split of final deman'!$G$17</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="12">'[1]Technology split of final deman'!$G$13</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="15">'[1]Technology split of final deman'!$G$13</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="14">'[1]Technology split of final deman'!$G$13</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="13">'[1]Technology split of final deman'!$G$13</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Coal_Heater" localSheetId="16">'[1]Technology split of final deman'!$G$13</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="12">'[1]Technology split of final deman'!$G$16</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="15">'[1]Technology split of final deman'!$G$16</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="14">'[1]Technology split of final deman'!$G$16</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="13">'[1]Technology split of final deman'!$G$16</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_District_Heating" localSheetId="16">'[1]Technology split of final deman'!$G$16</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="12">'[1]Technology split of final deman'!$G$11</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="15">'[1]Technology split of final deman'!$G$11</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="14">'[1]Technology split of final deman'!$G$11</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="13">'[1]Technology split of final deman'!$G$11</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heat_Pump" localSheetId="16">'[1]Technology split of final deman'!$G$11</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="12">'[1]Technology split of final deman'!$G$12</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="15">'[1]Technology split of final deman'!$G$12</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="14">'[1]Technology split of final deman'!$G$12</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="13">'[1]Technology split of final deman'!$G$12</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Elec_Heater" localSheetId="16">'[1]Technology split of final deman'!$G$12</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="12">'[1]Technology split of final deman'!$G$10</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="15">'[1]Technology split of final deman'!$G$10</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="14">'[1]Technology split of final deman'!$G$10</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="13">'[1]Technology split of final deman'!$G$10</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heat_Pump" localSheetId="16">'[1]Technology split of final deman'!$G$10</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="12">'[1]Technology split of final deman'!$G$9</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="15">'[1]Technology split of final deman'!$G$9</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="14">'[1]Technology split of final deman'!$G$9</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="13">'[1]Technology split of final deman'!$G$9</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Gas_Heater" localSheetId="16">'[1]Technology split of final deman'!$G$9</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="12">'[1]Technology split of final deman'!$G$14</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="15">'[1]Technology split of final deman'!$G$14</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="14">'[1]Technology split of final deman'!$G$14</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="13">'[1]Technology split of final deman'!$G$14</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Oil_Heater" localSheetId="16">'[1]Technology split of final deman'!$G$14</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="12">'[1]Technology split of final deman'!$G$18</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="15">'[1]Technology split of final deman'!$G$18</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="14">'[1]Technology split of final deman'!$G$18</definedName>
     <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="13">'[1]Technology split of final deman'!$G$18</definedName>
+    <definedName name="Perc_Final_Demand_Space_Heating_Solar_Heater" localSheetId="16">'[1]Technology split of final deman'!$G$18</definedName>
     <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="12">'[1]Tech split of useful demand'!$G$17</definedName>
     <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="15">'[1]Tech split of useful demand'!$G$17</definedName>
     <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="14">'[1]Tech split of useful demand'!$G$17</definedName>
     <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="13">'[1]Tech split of useful demand'!$G$17</definedName>
+    <definedName name="Perc_Heat_Delivered_Biomass_Heater" localSheetId="16">'[1]Tech split of useful demand'!$G$17</definedName>
     <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="12">'[1]Tech split of useful demand'!$G$16</definedName>
     <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="15">'[1]Tech split of useful demand'!$G$16</definedName>
     <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="14">'[1]Tech split of useful demand'!$G$16</definedName>
     <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="13">'[1]Tech split of useful demand'!$G$16</definedName>
+    <definedName name="Perc_Heat_Delivered_District_Heat" localSheetId="16">'[1]Tech split of useful demand'!$G$16</definedName>
     <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="12">'[1]Tech split of useful demand'!$G$18</definedName>
     <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="15">'[1]Tech split of useful demand'!$G$18</definedName>
     <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="14">'[1]Tech split of useful demand'!$G$18</definedName>
     <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="13">'[1]Tech split of useful demand'!$G$18</definedName>
+    <definedName name="Perc_Heat_Delivered_Solar_Thermal" localSheetId="16">'[1]Tech split of useful demand'!$G$18</definedName>
     <definedName name="Perc_Roof_for_PV" localSheetId="12">'[1]PV solar area and production'!$E$22</definedName>
     <definedName name="Perc_Roof_for_PV" localSheetId="15">'[1]PV solar area and production'!$E$22</definedName>
     <definedName name="Perc_Roof_for_PV" localSheetId="14">'[1]PV solar area and production'!$E$22</definedName>
     <definedName name="Perc_Roof_for_PV" localSheetId="13">'[1]PV solar area and production'!$E$22</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="Perc_Roof_for_PV" localSheetId="16">'[1]PV solar area and production'!$E$22</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_carbothermal_reduction" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_carbothermal_reduction">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_bat" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_bat" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_bat">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_electrolysis_current" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_electrolysis_current" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_electrolysis_current">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_aluminium_melting_oven" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_aluminium_melting_oven" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_aluminium_melting_oven">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_coal_gas" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_coal_gas">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_blast_furnace_burner_network_gas" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_blast_furnace_burner_network_gas">Dashboard!#REF!</definedName>
     <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="12">'[1]Shares per tech per carrier'!$E$22</definedName>
     <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="15">'[1]Shares per tech per carrier'!$E$22</definedName>
     <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="14">'[1]Shares per tech per carrier'!$E$22</definedName>
     <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="13">'[1]Shares per tech per carrier'!$E$22</definedName>
+    <definedName name="Share_Lighting_Fluorescent_Lamp" localSheetId="16">'[1]Shares per tech per carrier'!$E$22</definedName>
     <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="12">'[1]Shares per tech per carrier'!$E$23</definedName>
     <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="15">'[1]Shares per tech per carrier'!$E$23</definedName>
     <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="14">'[1]Shares per tech per carrier'!$E$23</definedName>
     <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="13">'[1]Shares per tech per carrier'!$E$23</definedName>
+    <definedName name="Share_Lighting_Fluorescent_Tube" localSheetId="16">'[1]Shares per tech per carrier'!$E$23</definedName>
     <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="12">'[1]Shares per tech per carrier'!$E$21</definedName>
     <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="15">'[1]Shares per tech per carrier'!$E$21</definedName>
     <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="14">'[1]Shares per tech per carrier'!$E$21</definedName>
     <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="13">'[1]Shares per tech per carrier'!$E$21</definedName>
+    <definedName name="Share_Lighting_Incandescent_Lamp" localSheetId="16">'[1]Shares per tech per carrier'!$E$21</definedName>
     <definedName name="Share_Lighting_LED" localSheetId="12">'[1]Shares per tech per carrier'!$E$24</definedName>
     <definedName name="Share_Lighting_LED" localSheetId="15">'[1]Shares per tech per carrier'!$E$24</definedName>
     <definedName name="Share_Lighting_LED" localSheetId="14">'[1]Shares per tech per carrier'!$E$24</definedName>
     <definedName name="Share_Lighting_LED" localSheetId="13">'[1]Shares per tech per carrier'!$E$24</definedName>
+    <definedName name="Share_Lighting_LED" localSheetId="16">'[1]Shares per tech per carrier'!$E$24</definedName>
     <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="12">'[1]Shares per tech per carrier'!$E$18</definedName>
     <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="15">'[1]Shares per tech per carrier'!$E$18</definedName>
     <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="14">'[1]Shares per tech per carrier'!$E$18</definedName>
     <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="13">'[1]Shares per tech per carrier'!$E$18</definedName>
+    <definedName name="Share_Space_Cooling_Electric_Airco" localSheetId="16">'[1]Shares per tech per carrier'!$E$18</definedName>
     <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="12">'[1]Shares per tech per carrier'!$E$17</definedName>
     <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="15">'[1]Shares per tech per carrier'!$E$17</definedName>
     <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="14">'[1]Shares per tech per carrier'!$E$17</definedName>
     <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="13">'[1]Shares per tech per carrier'!$E$17</definedName>
+    <definedName name="Share_Space_Cooling_Electric_Heat_Pump" localSheetId="16">'[1]Shares per tech per carrier'!$E$17</definedName>
     <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="12">'[1]Shares per tech per carrier'!$E$13</definedName>
     <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="15">'[1]Shares per tech per carrier'!$E$13</definedName>
     <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="14">'[1]Shares per tech per carrier'!$E$13</definedName>
     <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="13">'[1]Shares per tech per carrier'!$E$13</definedName>
+    <definedName name="Share_Space_Heating_Electric_Heat_Pump" localSheetId="16">'[1]Shares per tech per carrier'!$E$13</definedName>
     <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="12">'[1]Shares per tech per carrier'!$E$14</definedName>
     <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="15">'[1]Shares per tech per carrier'!$E$14</definedName>
     <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="14">'[1]Shares per tech per carrier'!$E$14</definedName>
     <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="13">'[1]Shares per tech per carrier'!$E$14</definedName>
+    <definedName name="Share_Space_Heating_Electric_Heater" localSheetId="16">'[1]Shares per tech per carrier'!$E$14</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="12">'[1]Shares per tech per carrier'!$E$10</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="15">'[1]Shares per tech per carrier'!$E$10</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="14">'[1]Shares per tech per carrier'!$E$10</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="13">'[1]Shares per tech per carrier'!$E$10</definedName>
+    <definedName name="Share_Space_Heating_Network_Gas_Heat_Pump" localSheetId="16">'[1]Shares per tech per carrier'!$E$10</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="12">'[1]Shares per tech per carrier'!$E$9</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="15">'[1]Shares per tech per carrier'!$E$9</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="14">'[1]Shares per tech per carrier'!$E$9</definedName>
     <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="13">'[1]Shares per tech per carrier'!$E$9</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="Share_Space_Heating_Network_Gas_Heater" localSheetId="16">'[1]Shares per tech per carrier'!$E$9</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_bat" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_bat" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_bat">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_blast_furnace_current" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_blast_furnace_current" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_steel_blast_furnace_current">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_cyclone" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_cyclone" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_steel_cyclone">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="share_steel_electric" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="share_steel_electric" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="share_steel_electric">Dashboard!#REF!</definedName>
     <definedName name="Solar_PV_Roof_CaPS" localSheetId="12">'[1]PV solar area and production'!$E$13</definedName>
     <definedName name="Solar_PV_Roof_CaPS" localSheetId="15">'[1]PV solar area and production'!$E$13</definedName>
     <definedName name="Solar_PV_Roof_CaPS" localSheetId="14">'[1]PV solar area and production'!$E$13</definedName>
     <definedName name="Solar_PV_Roof_CaPS" localSheetId="13">'[1]PV solar area and production'!$E$13</definedName>
+    <definedName name="Solar_PV_Roof_CaPS" localSheetId="16">'[1]PV solar area and production'!$E$13</definedName>
     <definedName name="Solar_PV_Roof_Residential" localSheetId="12">'[1]IEA autoproducer prod.'!$AO$10</definedName>
     <definedName name="Solar_PV_Roof_Residential" localSheetId="15">'[1]IEA autoproducer prod.'!$AO$10</definedName>
     <definedName name="Solar_PV_Roof_Residential" localSheetId="14">'[1]IEA autoproducer prod.'!$AO$10</definedName>
     <definedName name="Solar_PV_Roof_Residential" localSheetId="13">'[1]IEA autoproducer prod.'!$AO$10</definedName>
+    <definedName name="Solar_PV_Roof_Residential" localSheetId="16">'[1]IEA autoproducer prod.'!$AO$10</definedName>
     <definedName name="Solar_PV_Roof_Total" localSheetId="12">'[1]Corrected energy balance'!$BG$95</definedName>
     <definedName name="Solar_PV_Roof_Total" localSheetId="15">'[1]Corrected energy balance'!$BG$95</definedName>
     <definedName name="Solar_PV_Roof_Total" localSheetId="14">'[1]Corrected energy balance'!$BG$95</definedName>
     <definedName name="Solar_PV_Roof_Total" localSheetId="13">'[1]Corrected energy balance'!$BG$95</definedName>
+    <definedName name="Solar_PV_Roof_Total" localSheetId="16">'[1]Corrected energy balance'!$BG$95</definedName>
     <definedName name="solver_adj" localSheetId="6" hidden="1">Dashboard!#REF!</definedName>
     <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="6" hidden="1">1</definedName>
@@ -556,22 +641,24 @@
     <definedName name="solver_typ" localSheetId="6" hidden="1">3</definedName>
     <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="6" hidden="1">2</definedName>
-    <definedName name="steel_production" localSheetId="17">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="24">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="20">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="26">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="23">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="19">Dashboard!#REF!</definedName>
-    <definedName name="steel_production" localSheetId="25">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="22">Dashboard!#REF!</definedName>
-    <definedName name="steel_production" localSheetId="24">Dashboard!#REF!</definedName>
-    <definedName name="steel_production" localSheetId="18">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="27">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="21">Dashboard!#REF!</definedName>
-    <definedName name="steel_production" localSheetId="26">Dashboard!#REF!</definedName>
-    <definedName name="steel_production" localSheetId="20">Dashboard!#REF!</definedName>
-    <definedName name="steel_production" localSheetId="27">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="28">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="29">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="15">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="14">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="13">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="10">Dashboard!#REF!</definedName>
     <definedName name="steel_production" localSheetId="11">Dashboard!#REF!</definedName>
+    <definedName name="steel_production" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="steel_production">Dashboard!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
@@ -607,7 +694,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="464">
   <si>
     <t>Changelog</t>
   </si>
@@ -1962,10 +2049,43 @@
     <t xml:space="preserve">On this sheet the input and output of oil carriers from refineries from the Energy Balance are aggregated. </t>
   </si>
   <si>
-    <t>In this sheet, the refinery efficiency is calculated for this dataset. The non-energetic crude oil and useable heat demand together make up the input. The output is equal to the sum of all refinery products. The loss is equal to the useable heat input plus the oil input minus oil output. This means that if the oil output is larger than the oil input, the efficiency exceeds 100%. If this efficiency were to be capped at 100%, however, this would mean fewer refinery products than reported will be produced. For that reason the effiency is not capped. The input and output conversions ('shares') are then exported as a csv.</t>
-  </si>
-  <si>
     <t>Overview of energetic and non-energetic final consumption in the Chemical industry. This data is exported to the Industry analysis using the purple export_to_industry_analysis sheet. The total non-energetic final consumption for non-energetic crude oil is corrected for the oil products which refineries produce for the petrochemical industry. The 'Cokes' column is included to ensure compatability with the Industry analysis. Cokes is not considered as a separate carrier, but aggregated in coal in this analysis.</t>
+  </si>
+  <si>
+    <t>In this sheet, the refinery efficiency is calculated for this dataset. The non-energetic crude oil and useable heat demand together make up the input. The output is equal to the sum of all refinery products. The loss is equal to the useable heat input plus the oil input minus oil output. This means that if the oil output is larger than the oil input, the efficiency exceeds 100%. If this efficiency were to be capped at 100%, however, this would mean fewer refinery products than reported will be produced. For that reason the efficiency is not capped. The input and output conversions ('shares') are then exported as a csv.</t>
+  </si>
+  <si>
+    <t>Network gas non energetic</t>
+  </si>
+  <si>
+    <t>Steam methane reformer input</t>
+  </si>
+  <si>
+    <t>On this page the fuel input for the steam methane reformer is determined.</t>
+  </si>
+  <si>
+    <t>Added steam methane reformer inputs sheets</t>
+  </si>
+  <si>
+    <t>Overview of oil input and oil products output of the refineries</t>
+  </si>
+  <si>
+    <t>Determination of heat production of refineries</t>
+  </si>
+  <si>
+    <t>An overview of the oil and heat input as well as the oil products output of the refinery</t>
+  </si>
+  <si>
+    <t>Determination of the input shares of heat and natural gas to the steam methane reformer in the fertilizers industry</t>
+  </si>
+  <si>
+    <t>csv_steam_methane_reformer_eff</t>
+  </si>
+  <si>
+    <t>input.network_gas</t>
+  </si>
+  <si>
+    <t>industry_chemicals_fertilizers_steam_methane_reformer_hydrogen_efficiency</t>
   </si>
 </sst>
 </file>
@@ -2819,7 +2939,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2025">
+  <cellStyleXfs count="2059">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4845,8 +4965,42 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="349">
+  <cellXfs count="351">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5534,8 +5688,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2025">
+  <cellStyles count="2059">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -6548,6 +6708,23 @@
     <cellStyle name="Followed Hyperlink" xfId="2020" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2022" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2026" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2028" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2030" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2032" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2034" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2036" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2038" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2040" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2042" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2044" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2046" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2048" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2050" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2052" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2054" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2056" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2058" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -7558,11 +7735,54 @@
     <cellStyle name="Hyperlink" xfId="2019" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2021" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2023" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2025" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2027" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2029" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2031" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2033" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2035" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2037" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2039" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2041" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2043" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2045" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2047" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2049" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2051" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2053" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2055" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2057" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="772"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -11389,7 +11609,7 @@
       </c>
       <c r="C5" s="19">
         <f>MAX(Changelog!D:D)</f>
-        <v>1.05</v>
+        <v>1.06</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -11419,7 +11639,7 @@
       </c>
       <c r="C8" s="76">
         <f>MAX(Changelog!B:B)</f>
-        <v>42594</v>
+        <v>42615</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -11706,7 +11926,7 @@
     <row r="5" spans="1:17" ht="113" customHeight="1">
       <c r="A5" s="82"/>
       <c r="B5" s="343" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C5" s="344"/>
       <c r="D5" s="344"/>
@@ -12507,7 +12727,7 @@
     <mergeCell ref="B5:E5"/>
   </mergeCells>
   <conditionalFormatting sqref="C19:K19">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13618,7 +13838,7 @@
     <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D44:E44">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14591,7 +14811,7 @@
     <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="D29:E29">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15275,7 +15495,7 @@
     <mergeCell ref="B5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="E26:M26">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15492,7 +15712,7 @@
     <mergeCell ref="B5:H5"/>
   </mergeCells>
   <conditionalFormatting sqref="E12:L12">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15721,7 +15941,7 @@
     <mergeCell ref="B5:F5"/>
   </mergeCells>
   <conditionalFormatting sqref="E16:I16">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15742,8 +15962,8 @@
   </sheetPr>
   <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15782,14 +16002,14 @@
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="84" customHeight="1">
       <c r="B5" s="346" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C5" s="347"/>
       <c r="D5" s="347"/>
@@ -16022,11 +16242,257 @@
     <mergeCell ref="B5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="5" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="B2:H21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="82"/>
+    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
+    <col min="5" max="11" width="15.83203125" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="82"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="20">
+      <c r="B2" s="81" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="2:8">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="8"/>
+    </row>
+    <row r="5" spans="2:8" ht="24" customHeight="1">
+      <c r="B5" s="346" t="s">
+        <v>455</v>
+      </c>
+      <c r="C5" s="347"/>
+      <c r="D5" s="347"/>
+      <c r="E5" s="347"/>
+      <c r="F5" s="347"/>
+      <c r="G5" s="348"/>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="2:8" ht="16" thickBot="1"/>
+    <row r="7" spans="2:8">
+      <c r="B7" s="138" t="s">
+        <v>208</v>
+      </c>
+      <c r="C7" s="107"/>
+      <c r="D7" s="139"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="325"/>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8" s="131"/>
+      <c r="C8" s="110"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="111"/>
+    </row>
+    <row r="9" spans="2:8">
+      <c r="B9" s="132" t="s">
+        <v>429</v>
+      </c>
+      <c r="C9" s="219"/>
+      <c r="D9" s="141"/>
+      <c r="E9" s="112" t="s">
+        <v>440</v>
+      </c>
+      <c r="F9" s="129" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8">
+      <c r="B10" s="135" t="s">
+        <v>446</v>
+      </c>
+      <c r="C10" s="246"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="167"/>
+      <c r="F10" s="168"/>
+    </row>
+    <row r="11" spans="2:8">
+      <c r="B11" s="135"/>
+      <c r="C11" s="246" t="s">
+        <v>190</v>
+      </c>
+      <c r="D11" s="143"/>
+      <c r="E11" s="167" t="e">
+        <f>Dashboard!E42*technical_specs!G12</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F11" s="334"/>
+    </row>
+    <row r="12" spans="2:8">
+      <c r="B12" s="134"/>
+      <c r="C12" s="246" t="s">
+        <v>209</v>
+      </c>
+      <c r="D12" s="143"/>
+      <c r="E12" s="167" t="e">
+        <f>Dashboard!E43*technical_specs!G15</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F12" s="334"/>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="134"/>
+      <c r="C13" s="246" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="143"/>
+      <c r="E13" s="167" t="e">
+        <f>Dashboard!E44*technical_specs!G13</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F13" s="334"/>
+    </row>
+    <row r="14" spans="2:8">
+      <c r="B14" s="134"/>
+      <c r="C14" s="246" t="s">
+        <v>192</v>
+      </c>
+      <c r="D14" s="143"/>
+      <c r="E14" s="167" t="e">
+        <f>Dashboard!E45*technical_specs!G14</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="334"/>
+    </row>
+    <row r="15" spans="2:8">
+      <c r="B15" s="134"/>
+      <c r="C15" s="246" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="143"/>
+      <c r="E15" s="167" t="str">
+        <f>Dashboard!E46</f>
+        <v/>
+      </c>
+      <c r="F15" s="334"/>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="134"/>
+      <c r="C16" s="246"/>
+      <c r="D16" s="143"/>
+      <c r="E16" s="167"/>
+      <c r="F16" s="334"/>
+    </row>
+    <row r="17" spans="2:6">
+      <c r="B17" s="318"/>
+      <c r="C17" s="349"/>
+      <c r="D17" s="320"/>
+      <c r="E17" s="321"/>
+      <c r="F17" s="350"/>
+    </row>
+    <row r="18" spans="2:6">
+      <c r="B18" s="135" t="s">
+        <v>430</v>
+      </c>
+      <c r="C18" s="246"/>
+      <c r="D18" s="143"/>
+      <c r="E18" s="167"/>
+      <c r="F18" s="168"/>
+    </row>
+    <row r="19" spans="2:6">
+      <c r="B19" s="135"/>
+      <c r="C19" s="246" t="s">
+        <v>453</v>
+      </c>
+      <c r="D19" s="143"/>
+      <c r="E19" s="167" t="str">
+        <f>Dashboard!E51</f>
+        <v/>
+      </c>
+      <c r="F19" s="324" t="e">
+        <f>IF(SUM($E$19:$E$20)=0,1,E19/SUM($E$19:$E$20))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6">
+      <c r="B20" s="135"/>
+      <c r="C20" s="246" t="s">
+        <v>431</v>
+      </c>
+      <c r="D20" s="143"/>
+      <c r="E20" s="167" t="e">
+        <f>SUM(E11:E15)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F20" s="324" t="e">
+        <f>IF(SUM($E$19:$E$20)=0,0,E20/SUM($E$19:$E$20))</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="16" thickBot="1">
+      <c r="B21" s="137"/>
+      <c r="C21" s="223"/>
+      <c r="D21" s="146"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="99"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B5:G5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F21">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -16041,7 +16507,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -16217,7 +16683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -16361,7 +16827,149 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
+    <tabColor theme="2"/>
+  </sheetPr>
+  <dimension ref="B2:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="90" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" ht="20">
+      <c r="B2" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="286" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="152" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="6"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="153"/>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="77">
+        <v>41583</v>
+      </c>
+      <c r="C6" s="118" t="s">
+        <v>274</v>
+      </c>
+      <c r="D6" s="119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="30">
+      <c r="B7" s="77">
+        <v>41611</v>
+      </c>
+      <c r="C7" s="122" t="s">
+        <v>296</v>
+      </c>
+      <c r="D7" s="128">
+        <v>1.01</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8" s="77">
+        <v>41618</v>
+      </c>
+      <c r="C8" s="121" t="s">
+        <v>297</v>
+      </c>
+      <c r="D8" s="128">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9" s="120">
+        <v>41682</v>
+      </c>
+      <c r="C9" s="121" t="s">
+        <v>308</v>
+      </c>
+      <c r="D9" s="128">
+        <v>1.03</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="30">
+      <c r="B10" s="120">
+        <v>42576</v>
+      </c>
+      <c r="C10" s="122" t="s">
+        <v>407</v>
+      </c>
+      <c r="D10" s="128">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="30">
+      <c r="B11" s="120">
+        <v>42594</v>
+      </c>
+      <c r="C11" s="122" t="s">
+        <v>449</v>
+      </c>
+      <c r="D11" s="128">
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4">
+      <c r="B12" s="120">
+        <v>42615</v>
+      </c>
+      <c r="C12" s="122" t="s">
+        <v>456</v>
+      </c>
+      <c r="D12" s="128">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4">
+      <c r="B13" s="120"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="128"/>
+    </row>
+    <row r="14" spans="2:4">
+      <c r="B14" s="13"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="154"/>
+    </row>
+    <row r="16" spans="2:4">
+      <c r="C16" s="121"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -16505,138 +17113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
-    <tabColor theme="2"/>
-  </sheetPr>
-  <dimension ref="B2:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="90" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:4" ht="20">
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4" s="286" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="152" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5" s="6"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="153"/>
-    </row>
-    <row r="6" spans="2:4">
-      <c r="B6" s="77">
-        <v>41583</v>
-      </c>
-      <c r="C6" s="118" t="s">
-        <v>274</v>
-      </c>
-      <c r="D6" s="119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="30">
-      <c r="B7" s="77">
-        <v>41611</v>
-      </c>
-      <c r="C7" s="122" t="s">
-        <v>296</v>
-      </c>
-      <c r="D7" s="128">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4">
-      <c r="B8" s="77">
-        <v>41618</v>
-      </c>
-      <c r="C8" s="121" t="s">
-        <v>297</v>
-      </c>
-      <c r="D8" s="128">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4">
-      <c r="B9" s="120">
-        <v>41682</v>
-      </c>
-      <c r="C9" s="121" t="s">
-        <v>308</v>
-      </c>
-      <c r="D9" s="128">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" ht="30">
-      <c r="B10" s="120">
-        <v>42576</v>
-      </c>
-      <c r="C10" s="122" t="s">
-        <v>407</v>
-      </c>
-      <c r="D10" s="128">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" ht="30">
-      <c r="B11" s="120">
-        <v>42594</v>
-      </c>
-      <c r="C11" s="122" t="s">
-        <v>449</v>
-      </c>
-      <c r="D11" s="128">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4">
-      <c r="B12" s="120"/>
-      <c r="C12" s="122"/>
-      <c r="D12" s="128"/>
-    </row>
-    <row r="13" spans="2:4">
-      <c r="B13" s="13"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="154"/>
-    </row>
-    <row r="15" spans="2:4">
-      <c r="C15" s="121"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet18" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -16780,7 +17257,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -16924,7 +17401,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17068,7 +17545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17212,7 +17689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17356,7 +17833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet23" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17500,7 +17977,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet24" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17638,7 +18115,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet25" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17782,7 +18259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet26" enableFormatConditionsCalculation="0">
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -17958,10 +18435,10 @@
   <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
     <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="B2:C29"/>
+  <dimension ref="B2:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18090,100 +18567,275 @@
       </c>
     </row>
     <row r="18" spans="2:3" ht="30" customHeight="1">
-      <c r="B18" s="97" t="s">
-        <v>255</v>
-      </c>
-      <c r="C18" s="150" t="s">
-        <v>226</v>
+      <c r="B18" s="95" t="s">
+        <v>417</v>
+      </c>
+      <c r="C18" s="149" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" customHeight="1">
-      <c r="B19" s="97" t="s">
-        <v>380</v>
-      </c>
-      <c r="C19" s="150" t="s">
-        <v>381</v>
+      <c r="B19" s="95" t="s">
+        <v>428</v>
+      </c>
+      <c r="C19" s="149" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" customHeight="1">
-      <c r="B20" s="97" t="s">
-        <v>382</v>
+      <c r="B20" s="96" t="s">
+        <v>441</v>
       </c>
       <c r="C20" s="150" t="s">
-        <v>383</v>
+        <v>459</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" customHeight="1">
-      <c r="B21" s="97" t="s">
-        <v>384</v>
+      <c r="B21" s="96" t="s">
+        <v>454</v>
       </c>
       <c r="C21" s="150" t="s">
-        <v>385</v>
+        <v>460</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" customHeight="1">
       <c r="B22" s="97" t="s">
-        <v>386</v>
+        <v>255</v>
       </c>
       <c r="C22" s="150" t="s">
-        <v>387</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30" customHeight="1">
       <c r="B23" s="97" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="C23" s="150" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="30" customHeight="1">
       <c r="B24" s="97" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C24" s="150" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="30" customHeight="1">
       <c r="B25" s="97" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C25" s="150" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="30" customHeight="1">
       <c r="B26" s="97" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
       <c r="C26" s="150" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="30" customHeight="1">
       <c r="B27" s="97" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C27" s="150" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="30" customHeight="1">
       <c r="B28" s="97" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="C28" s="150" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="30" customHeight="1">
       <c r="B29" s="97" t="s">
+        <v>392</v>
+      </c>
+      <c r="C29" s="150" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="30" customHeight="1">
+      <c r="B30" s="97" t="s">
+        <v>395</v>
+      </c>
+      <c r="C30" s="150" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="30" customHeight="1">
+      <c r="B31" s="97" t="s">
+        <v>396</v>
+      </c>
+      <c r="C31" s="150" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="30" customHeight="1">
+      <c r="B32" s="97" t="s">
+        <v>398</v>
+      </c>
+      <c r="C32" s="150" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="30" customHeight="1">
+      <c r="B33" s="97" t="s">
         <v>443</v>
       </c>
-      <c r="C29" s="150" t="s">
+      <c r="C33" s="150" t="s">
         <v>444</v>
       </c>
+    </row>
+    <row r="34" spans="2:3" ht="30" customHeight="1">
+      <c r="B34" s="97" t="s">
+        <v>461</v>
+      </c>
+      <c r="C34" s="150" t="s">
+        <v>444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="27" style="277" customWidth="1"/>
+    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="277" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="277" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="277" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="278" t="s">
+        <v>462</v>
+      </c>
+      <c r="B3" s="317" t="e">
+        <f>'Steam methane reformer input'!F19</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="278" t="s">
+        <v>427</v>
+      </c>
+      <c r="B4" s="317" t="e">
+        <f>'Steam methane reformer input'!F20</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="B5" s="317"/>
+      <c r="C5" s="296"/>
+      <c r="D5" s="193"/>
+      <c r="E5" s="193"/>
+      <c r="F5" s="193"/>
+      <c r="G5" s="193"/>
+      <c r="H5" s="193"/>
+      <c r="I5" s="193"/>
+      <c r="J5" s="193"/>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="278"/>
+      <c r="B6" s="317"/>
+      <c r="C6" s="296"/>
+      <c r="D6" s="296"/>
+      <c r="E6" s="296"/>
+      <c r="F6" s="296"/>
+      <c r="G6" s="296"/>
+      <c r="H6" s="296"/>
+      <c r="I6" s="296"/>
+      <c r="J6" s="296"/>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="278"/>
+      <c r="B7" s="317"/>
+      <c r="C7" s="296"/>
+      <c r="D7" s="296"/>
+      <c r="E7" s="296"/>
+      <c r="F7" s="296"/>
+      <c r="G7" s="296"/>
+      <c r="H7" s="296"/>
+      <c r="I7" s="296"/>
+      <c r="J7" s="296"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="278"/>
+      <c r="B8" s="317"/>
+      <c r="C8" s="193"/>
+      <c r="D8" s="193"/>
+      <c r="E8" s="193"/>
+      <c r="F8" s="193"/>
+      <c r="G8" s="193"/>
+      <c r="H8" s="193"/>
+      <c r="I8" s="193"/>
+      <c r="J8" s="193"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="278"/>
+      <c r="B9" s="317"/>
+      <c r="C9" s="296"/>
+      <c r="D9" s="193"/>
+      <c r="E9" s="193"/>
+      <c r="F9" s="193"/>
+      <c r="G9" s="193"/>
+      <c r="H9" s="193"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="193"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="278"/>
+      <c r="B10" s="317"/>
+      <c r="C10" s="296"/>
+      <c r="D10" s="301"/>
+      <c r="E10" s="193"/>
+      <c r="F10" s="193"/>
+      <c r="G10" s="193"/>
+      <c r="H10" s="193"/>
+      <c r="I10" s="193"/>
+      <c r="J10" s="193"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="278"/>
+      <c r="B11" s="317"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20242,7 +20894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" hidden="1" outlineLevel="1">
+    <row r="39" spans="1:16" outlineLevel="1">
       <c r="A39" s="8"/>
       <c r="B39" s="31"/>
       <c r="C39" s="257"/>
@@ -20260,7 +20912,7 @@
       <c r="O39" s="207"/>
       <c r="P39" s="208"/>
     </row>
-    <row r="40" spans="1:16" hidden="1" outlineLevel="1">
+    <row r="40" spans="1:16" outlineLevel="1">
       <c r="A40" s="8"/>
       <c r="B40" s="28" t="s">
         <v>310</v>
@@ -20280,7 +20932,7 @@
       <c r="O40" s="207"/>
       <c r="P40" s="208"/>
     </row>
-    <row r="41" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="41" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A41" s="8"/>
       <c r="B41" s="22" t="s">
         <v>283</v>
@@ -20300,7 +20952,7 @@
       <c r="O41" s="207"/>
       <c r="P41" s="208"/>
     </row>
-    <row r="42" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="42" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A42" s="8"/>
       <c r="B42" s="22"/>
       <c r="C42" s="258" t="s">
@@ -20335,7 +20987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="43" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A43" s="8"/>
       <c r="B43" s="22"/>
       <c r="C43" s="258" t="s">
@@ -20370,7 +21022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="44" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A44" s="8"/>
       <c r="B44" s="22"/>
       <c r="C44" s="258" t="s">
@@ -20405,7 +21057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="45" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A45" s="8"/>
       <c r="B45" s="22"/>
       <c r="C45" s="258" t="s">
@@ -20440,7 +21092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="46" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A46" s="8"/>
       <c r="B46" s="22"/>
       <c r="C46" s="258" t="s">
@@ -20475,7 +21127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="47" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A47" s="8"/>
       <c r="B47" s="22"/>
       <c r="C47" s="258" t="s">
@@ -20510,7 +21162,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" hidden="1" outlineLevel="1">
+    <row r="48" spans="1:16" outlineLevel="1">
       <c r="A48" s="8"/>
       <c r="B48" s="22"/>
       <c r="C48" s="202"/>
@@ -20528,7 +21180,7 @@
       <c r="O48" s="207"/>
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="49" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A49" s="8"/>
       <c r="B49" s="22" t="s">
         <v>284</v>
@@ -20548,7 +21200,7 @@
       <c r="O49" s="207"/>
       <c r="P49" s="208"/>
     </row>
-    <row r="50" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A50" s="8"/>
       <c r="B50" s="22"/>
       <c r="C50" s="258" t="s">
@@ -20583,7 +21235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="51" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A51" s="8"/>
       <c r="B51" s="22"/>
       <c r="C51" s="258" t="s">
@@ -20618,7 +21270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="16" hidden="1" outlineLevel="1" thickBot="1">
+    <row r="52" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
       <c r="A52" s="8"/>
       <c r="B52" s="22"/>
       <c r="C52" s="258" t="s">
@@ -20653,7 +21305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="16" collapsed="1" thickBot="1">
+    <row r="53" spans="1:16" ht="16" thickBot="1">
       <c r="B53" s="33"/>
       <c r="C53" s="46"/>
       <c r="D53" s="159"/>
@@ -20675,82 +21327,82 @@
     <mergeCell ref="B5:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="L18">
-    <cfRule type="cellIs" dxfId="23" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="19" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="cellIs" dxfId="22" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="17" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="cellIs" dxfId="20" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="19" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L34">
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L38">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L42">
-    <cfRule type="cellIs" dxfId="16" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43">
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L44">
-    <cfRule type="cellIs" dxfId="14" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L46">
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Published state of ETDataset on 2 November 2016
</commit_message>
<xml_diff>
--- a/analyses/4b_chemical_industry_analysis.xlsx
+++ b/analyses/4b_chemical_industry_analysis.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27526"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="23520" tabRatio="835" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="835" firstSheet="25" activeTab="28"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -2013,9 +2013,6 @@
     <t>Oil products</t>
   </si>
   <si>
-    <t>output.oil_products</t>
-  </si>
-  <si>
     <t>Total (TJ)</t>
   </si>
   <si>
@@ -2086,6 +2083,9 @@
   </si>
   <si>
     <t>industry_chemicals_fertilizers_steam_methane_reformer_hydrogen_efficiency</t>
+  </si>
+  <si>
+    <t>output.crude_oil</t>
   </si>
 </sst>
 </file>
@@ -5646,6 +5646,12 @@
     <xf numFmtId="167" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5687,12 +5693,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2059">
@@ -11580,16 +11580,16 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="13.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="1" customWidth="1"/>
-    <col min="4" max="7" width="10.83203125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="7" width="10.875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="20">
+    <row r="2" spans="2:4" ht="21">
       <c r="B2" s="2" t="s">
         <v>186</v>
       </c>
@@ -11685,14 +11685,14 @@
       </c>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="2:4" ht="16" thickBot="1">
+    <row r="15" spans="2:4" ht="17" thickBot="1">
       <c r="B15" s="14"/>
       <c r="C15" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="7"/>
     </row>
-    <row r="16" spans="2:4" ht="16" thickBot="1">
+    <row r="16" spans="2:4" ht="17" thickBot="1">
       <c r="B16" s="14"/>
       <c r="C16" s="16" t="s">
         <v>12</v>
@@ -11852,14 +11852,14 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" style="90" customWidth="1"/>
-    <col min="6" max="10" width="14.33203125" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="4" width="14.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.375" style="90" customWidth="1"/>
+    <col min="6" max="10" width="14.375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -11876,7 +11876,7 @@
       <c r="L1" s="82"/>
       <c r="M1" s="82"/>
     </row>
-    <row r="2" spans="1:17" ht="20">
+    <row r="2" spans="1:17" ht="21">
       <c r="A2" s="82"/>
       <c r="B2" s="81" t="s">
         <v>207</v>
@@ -11925,12 +11925,12 @@
     </row>
     <row r="5" spans="1:17" ht="113" customHeight="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="343" t="s">
-        <v>451</v>
-      </c>
-      <c r="C5" s="344"/>
-      <c r="D5" s="344"/>
-      <c r="E5" s="345"/>
+      <c r="B5" s="345" t="s">
+        <v>450</v>
+      </c>
+      <c r="C5" s="346"/>
+      <c r="D5" s="346"/>
+      <c r="E5" s="347"/>
       <c r="F5" s="82"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
@@ -11939,7 +11939,7 @@
       <c r="K5" s="82"/>
       <c r="L5" s="82"/>
     </row>
-    <row r="6" spans="1:17" ht="16" thickBot="1">
+    <row r="6" spans="1:17" ht="17" thickBot="1">
       <c r="A6" s="82"/>
       <c r="B6" s="82"/>
       <c r="C6" s="82"/>
@@ -11988,7 +11988,7 @@
       <c r="M8" s="82"/>
       <c r="N8" s="82"/>
     </row>
-    <row r="9" spans="1:17" ht="30">
+    <row r="9" spans="1:17">
       <c r="A9" s="82"/>
       <c r="B9" s="115"/>
       <c r="C9" s="155" t="s">
@@ -12025,7 +12025,7 @@
       <c r="P9" s="82"/>
       <c r="Q9" s="82"/>
     </row>
-    <row r="10" spans="1:17" ht="30">
+    <row r="10" spans="1:17" ht="32">
       <c r="A10" s="82"/>
       <c r="B10" s="106" t="s">
         <v>402</v>
@@ -12232,7 +12232,7 @@
       <c r="P14" s="82"/>
       <c r="Q14" s="82"/>
     </row>
-    <row r="15" spans="1:17" ht="30">
+    <row r="15" spans="1:17" ht="32">
       <c r="A15" s="82"/>
       <c r="B15" s="106" t="s">
         <v>403</v>
@@ -12421,7 +12421,7 @@
       <c r="P18" s="82"/>
       <c r="Q18" s="82"/>
     </row>
-    <row r="19" spans="1:17" ht="16" thickBot="1">
+    <row r="19" spans="1:17" ht="17" thickBot="1">
       <c r="A19" s="82"/>
       <c r="B19" s="114"/>
       <c r="C19" s="171"/>
@@ -12752,15 +12752,15 @@
       <selection activeCell="E11" sqref="E11:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="21.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="90" customWidth="1"/>
-    <col min="7" max="11" width="14.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="3" width="21.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="90" customWidth="1"/>
+    <col min="7" max="11" width="14.375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -12778,7 +12778,7 @@
       <c r="M1" s="82"/>
       <c r="N1" s="82"/>
     </row>
-    <row r="2" spans="1:14" ht="20">
+    <row r="2" spans="1:14" ht="21">
       <c r="A2" s="82"/>
       <c r="B2" s="81" t="s">
         <v>341</v>
@@ -12829,13 +12829,13 @@
     </row>
     <row r="5" spans="1:14" ht="41" customHeight="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="343" t="s">
+      <c r="B5" s="345" t="s">
         <v>335</v>
       </c>
-      <c r="C5" s="344"/>
-      <c r="D5" s="344"/>
-      <c r="E5" s="344"/>
-      <c r="F5" s="345"/>
+      <c r="C5" s="346"/>
+      <c r="D5" s="346"/>
+      <c r="E5" s="346"/>
+      <c r="F5" s="347"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
       <c r="I5" s="82"/>
@@ -12844,7 +12844,7 @@
       <c r="L5" s="82"/>
       <c r="M5" s="82"/>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1">
+    <row r="6" spans="1:14" ht="17" thickBot="1">
       <c r="A6" s="82"/>
       <c r="B6" s="82"/>
       <c r="C6" s="82"/>
@@ -13449,7 +13449,7 @@
       <c r="J39" s="82"/>
       <c r="K39" s="82"/>
     </row>
-    <row r="40" spans="1:17" ht="30">
+    <row r="40" spans="1:17" ht="32">
       <c r="A40" s="82"/>
       <c r="B40" s="304" t="s">
         <v>338</v>
@@ -13527,7 +13527,7 @@
       <c r="J43" s="82"/>
       <c r="K43" s="82"/>
     </row>
-    <row r="44" spans="1:17" ht="16" thickBot="1">
+    <row r="44" spans="1:17" ht="17" thickBot="1">
       <c r="A44" s="82"/>
       <c r="B44" s="137"/>
       <c r="C44" s="146"/>
@@ -13863,15 +13863,15 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="3" width="21.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="90" customWidth="1"/>
-    <col min="7" max="11" width="14.33203125" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="3" width="21.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.375" style="90" customWidth="1"/>
+    <col min="7" max="11" width="14.375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -13889,7 +13889,7 @@
       <c r="M1" s="82"/>
       <c r="N1" s="82"/>
     </row>
-    <row r="2" spans="1:14" ht="20">
+    <row r="2" spans="1:14" ht="21">
       <c r="A2" s="82"/>
       <c r="B2" s="81" t="s">
         <v>340</v>
@@ -13940,13 +13940,13 @@
     </row>
     <row r="5" spans="1:14" ht="41" customHeight="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="343" t="s">
+      <c r="B5" s="345" t="s">
         <v>339</v>
       </c>
-      <c r="C5" s="344"/>
-      <c r="D5" s="344"/>
-      <c r="E5" s="344"/>
-      <c r="F5" s="345"/>
+      <c r="C5" s="346"/>
+      <c r="D5" s="346"/>
+      <c r="E5" s="346"/>
+      <c r="F5" s="347"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
       <c r="I5" s="82"/>
@@ -13955,7 +13955,7 @@
       <c r="L5" s="82"/>
       <c r="M5" s="82"/>
     </row>
-    <row r="6" spans="1:14" ht="16" thickBot="1">
+    <row r="6" spans="1:14" ht="17" thickBot="1">
       <c r="A6" s="82"/>
       <c r="B6" s="82"/>
       <c r="C6" s="82"/>
@@ -14365,7 +14365,7 @@
       <c r="J28" s="82"/>
       <c r="K28" s="82"/>
     </row>
-    <row r="29" spans="1:11" ht="16" thickBot="1">
+    <row r="29" spans="1:11" ht="17" thickBot="1">
       <c r="A29" s="82"/>
       <c r="B29" s="137"/>
       <c r="C29" s="146"/>
@@ -14836,17 +14836,17 @@
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="82"/>
-    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
-    <col min="5" max="13" width="15.83203125" style="82" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="82"/>
+    <col min="1" max="1" width="10.625" style="82"/>
+    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
+    <col min="5" max="13" width="15.875" style="82" customWidth="1"/>
+    <col min="14" max="16384" width="10.625" style="82"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="20">
+    <row r="2" spans="2:13" ht="21">
       <c r="B2" s="81" t="s">
         <v>199</v>
       </c>
@@ -14878,17 +14878,17 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:13" ht="107" customHeight="1">
-      <c r="B5" s="346" t="s">
+      <c r="B5" s="348" t="s">
         <v>405</v>
       </c>
-      <c r="C5" s="347"/>
-      <c r="D5" s="347"/>
-      <c r="E5" s="347"/>
-      <c r="F5" s="347"/>
-      <c r="G5" s="348"/>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="349"/>
+      <c r="F5" s="349"/>
+      <c r="G5" s="350"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="2:13" ht="16" thickBot="1"/>
+    <row r="6" spans="2:13" ht="17" thickBot="1"/>
     <row r="7" spans="2:13">
       <c r="B7" s="138" t="s">
         <v>208</v>
@@ -15025,7 +15025,7 @@
       <c r="L12" s="217"/>
       <c r="M12" s="218"/>
     </row>
-    <row r="13" spans="2:13" ht="30">
+    <row r="13" spans="2:13">
       <c r="B13" s="135" t="s">
         <v>277</v>
       </c>
@@ -15263,7 +15263,7 @@
       <c r="L19" s="217"/>
       <c r="M19" s="218"/>
     </row>
-    <row r="20" spans="2:13" ht="30">
+    <row r="20" spans="2:13" ht="32">
       <c r="B20" s="135" t="s">
         <v>278</v>
       </c>
@@ -15476,7 +15476,7 @@
         <v>ERROR</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="16" thickBot="1">
+    <row r="26" spans="2:13" ht="17" thickBot="1">
       <c r="B26" s="137"/>
       <c r="C26" s="223"/>
       <c r="D26" s="146"/>
@@ -15520,17 +15520,17 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="82"/>
-    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
-    <col min="5" max="13" width="15.83203125" style="82" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="82"/>
+    <col min="1" max="1" width="10.625" style="82"/>
+    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
+    <col min="5" max="13" width="15.875" style="82" customWidth="1"/>
+    <col min="14" max="16384" width="10.625" style="82"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="20">
+    <row r="2" spans="2:12" ht="21">
       <c r="B2" s="81" t="s">
         <v>417</v>
       </c>
@@ -15565,18 +15565,18 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="2:12" ht="26" customHeight="1">
-      <c r="B5" s="346" t="s">
-        <v>450</v>
-      </c>
-      <c r="C5" s="347"/>
-      <c r="D5" s="347"/>
-      <c r="E5" s="347"/>
-      <c r="F5" s="347"/>
-      <c r="G5" s="347"/>
-      <c r="H5" s="348"/>
+      <c r="B5" s="348" t="s">
+        <v>449</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="349"/>
+      <c r="F5" s="349"/>
+      <c r="G5" s="349"/>
+      <c r="H5" s="350"/>
       <c r="I5" s="8"/>
     </row>
-    <row r="6" spans="2:12" ht="16" thickBot="1"/>
+    <row r="6" spans="2:12" ht="17" thickBot="1"/>
     <row r="7" spans="2:12">
       <c r="B7" s="138" t="s">
         <v>208</v>
@@ -15609,7 +15609,7 @@
       <c r="K8" s="110"/>
       <c r="L8" s="111"/>
     </row>
-    <row r="9" spans="2:12" ht="30">
+    <row r="9" spans="2:12" ht="32">
       <c r="B9" s="132" t="s">
         <v>261</v>
       </c>
@@ -15637,7 +15637,7 @@
         <v>416</v>
       </c>
       <c r="L9" s="129" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="10" spans="2:12">
@@ -15694,7 +15694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="16" thickBot="1">
+    <row r="12" spans="2:12" ht="17" thickBot="1">
       <c r="B12" s="137"/>
       <c r="C12" s="223"/>
       <c r="D12" s="146"/>
@@ -15737,17 +15737,17 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="82"/>
-    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
-    <col min="5" max="10" width="15.83203125" style="82" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="82"/>
+    <col min="1" max="1" width="10.625" style="82"/>
+    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
+    <col min="5" max="10" width="15.875" style="82" customWidth="1"/>
+    <col min="11" max="16384" width="10.625" style="82"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="20">
+    <row r="2" spans="2:9" ht="21">
       <c r="B2" s="81" t="s">
         <v>428</v>
       </c>
@@ -15776,16 +15776,16 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="2:9" ht="37" customHeight="1">
-      <c r="B5" s="346" t="s">
-        <v>448</v>
-      </c>
-      <c r="C5" s="347"/>
-      <c r="D5" s="347"/>
-      <c r="E5" s="347"/>
-      <c r="F5" s="348"/>
+      <c r="B5" s="348" t="s">
+        <v>447</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="349"/>
+      <c r="F5" s="350"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="2:9" ht="16" thickBot="1"/>
+    <row r="6" spans="2:9" ht="17" thickBot="1"/>
     <row r="7" spans="2:9">
       <c r="B7" s="138" t="s">
         <v>208</v>
@@ -15889,7 +15889,7 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="135" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C14" s="246"/>
       <c r="D14" s="143"/>
@@ -15926,7 +15926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" ht="16" thickBot="1">
+    <row r="16" spans="2:9" ht="17" thickBot="1">
       <c r="B16" s="137"/>
       <c r="C16" s="223"/>
       <c r="D16" s="146"/>
@@ -15966,19 +15966,19 @@
       <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="82"/>
-    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
-    <col min="5" max="11" width="15.83203125" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="82"/>
+    <col min="1" max="1" width="10.625" style="82"/>
+    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
+    <col min="5" max="11" width="15.875" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="10.625" style="82"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="20">
+    <row r="2" spans="2:8" ht="21">
       <c r="B2" s="81" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C2" s="81"/>
       <c r="D2" s="81"/>
@@ -16008,17 +16008,17 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="84" customHeight="1">
-      <c r="B5" s="346" t="s">
-        <v>452</v>
-      </c>
-      <c r="C5" s="347"/>
-      <c r="D5" s="347"/>
-      <c r="E5" s="347"/>
-      <c r="F5" s="347"/>
-      <c r="G5" s="348"/>
+      <c r="B5" s="348" t="s">
+        <v>451</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="349"/>
+      <c r="F5" s="349"/>
+      <c r="G5" s="350"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="2:8" ht="16" thickBot="1"/>
+    <row r="6" spans="2:8" ht="17" thickBot="1"/>
     <row r="7" spans="2:8">
       <c r="B7" s="138" t="s">
         <v>208</v>
@@ -16042,7 +16042,7 @@
       <c r="C9" s="219"/>
       <c r="D9" s="141"/>
       <c r="E9" s="112" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F9" s="129" t="s">
         <v>337</v>
@@ -16218,7 +16218,7 @@
     <row r="23" spans="2:6">
       <c r="B23" s="134"/>
       <c r="C23" s="326" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D23" s="143"/>
       <c r="E23" s="167">
@@ -16230,7 +16230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="16" thickBot="1">
+    <row r="24" spans="2:6" ht="17" thickBot="1">
       <c r="B24" s="137"/>
       <c r="C24" s="223"/>
       <c r="D24" s="146"/>
@@ -16272,19 +16272,19 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="82"/>
-    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
-    <col min="5" max="11" width="15.83203125" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="82"/>
+    <col min="1" max="1" width="10.625" style="82"/>
+    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
+    <col min="5" max="11" width="15.875" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="10.625" style="82"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="20">
+    <row r="2" spans="2:8" ht="21">
       <c r="B2" s="81" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C2" s="81"/>
       <c r="D2" s="81"/>
@@ -16314,17 +16314,17 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1">
-      <c r="B5" s="346" t="s">
-        <v>455</v>
-      </c>
-      <c r="C5" s="347"/>
-      <c r="D5" s="347"/>
-      <c r="E5" s="347"/>
-      <c r="F5" s="347"/>
-      <c r="G5" s="348"/>
+      <c r="B5" s="348" t="s">
+        <v>454</v>
+      </c>
+      <c r="C5" s="349"/>
+      <c r="D5" s="349"/>
+      <c r="E5" s="349"/>
+      <c r="F5" s="349"/>
+      <c r="G5" s="350"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="2:8" ht="16" thickBot="1"/>
+    <row r="6" spans="2:8" ht="17" thickBot="1"/>
     <row r="7" spans="2:8">
       <c r="B7" s="138" t="s">
         <v>208</v>
@@ -16348,7 +16348,7 @@
       <c r="C9" s="219"/>
       <c r="D9" s="141"/>
       <c r="E9" s="112" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F9" s="129" t="s">
         <v>337</v>
@@ -16356,7 +16356,7 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="135" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C10" s="246"/>
       <c r="D10" s="143"/>
@@ -16432,10 +16432,10 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="318"/>
-      <c r="C17" s="349"/>
+      <c r="C17" s="335"/>
       <c r="D17" s="320"/>
       <c r="E17" s="321"/>
-      <c r="F17" s="350"/>
+      <c r="F17" s="336"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="135" t="s">
@@ -16449,7 +16449,7 @@
     <row r="19" spans="2:6">
       <c r="B19" s="135"/>
       <c r="C19" s="246" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D19" s="143"/>
       <c r="E19" s="167" t="str">
@@ -16476,7 +16476,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="16" thickBot="1">
+    <row r="21" spans="2:6" ht="17" thickBot="1">
       <c r="B21" s="137"/>
       <c r="C21" s="223"/>
       <c r="D21" s="146"/>
@@ -16518,10 +16518,10 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -16694,10 +16694,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -16838,16 +16838,16 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="90" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="20.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="90" customWidth="1"/>
+    <col min="5" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="20">
+    <row r="2" spans="2:4" ht="21">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -16879,7 +16879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="30">
+    <row r="7" spans="2:4">
       <c r="B7" s="77">
         <v>41611</v>
       </c>
@@ -16912,7 +16912,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
+    <row r="10" spans="2:4" ht="32">
       <c r="B10" s="120">
         <v>42576</v>
       </c>
@@ -16923,12 +16923,12 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30">
+    <row r="11" spans="2:4">
       <c r="B11" s="120">
         <v>42594</v>
       </c>
       <c r="C11" s="122" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D11" s="128">
         <v>1.05</v>
@@ -16939,7 +16939,7 @@
         <v>42615</v>
       </c>
       <c r="C12" s="122" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D12" s="128">
         <v>1.06</v>
@@ -16980,10 +16980,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17124,10 +17124,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17268,10 +17268,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17412,10 +17412,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17556,10 +17556,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17700,10 +17700,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17844,10 +17844,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17988,11 +17988,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="54" style="277" customWidth="1"/>
-    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18126,10 +18126,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18266,15 +18266,15 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" style="277" customWidth="1"/>
-    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18412,7 +18412,7 @@
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="278" t="s">
-        <v>439</v>
+        <v>463</v>
       </c>
       <c r="B11" s="317">
         <f>'Refineries efficiency'!F22</f>
@@ -18441,15 +18441,15 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="35.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="100.83203125" style="116" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="35.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="100.875" style="116" customWidth="1"/>
+    <col min="4" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="20">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
@@ -18571,7 +18571,7 @@
         <v>417</v>
       </c>
       <c r="C18" s="149" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="30" customHeight="1">
@@ -18579,23 +18579,23 @@
         <v>428</v>
       </c>
       <c r="C19" s="149" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="30" customHeight="1">
       <c r="B20" s="96" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C20" s="150" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="30" customHeight="1">
       <c r="B21" s="96" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C21" s="150" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="30" customHeight="1">
@@ -18688,18 +18688,18 @@
     </row>
     <row r="33" spans="2:3" ht="30" customHeight="1">
       <c r="B33" s="97" t="s">
+        <v>442</v>
+      </c>
+      <c r="C33" s="150" t="s">
         <v>443</v>
-      </c>
-      <c r="C33" s="150" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="30" customHeight="1">
       <c r="B34" s="97" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C34" s="150" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -18724,16 +18724,16 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27" style="277" customWidth="1"/>
-    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11.625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="277" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -18746,7 +18746,7 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="278" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B3" s="317" t="e">
         <f>'Steam methane reformer input'!F19</f>
@@ -18857,14 +18857,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="140.83203125" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="140.875" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" ht="20">
+    <row r="2" spans="2:2" ht="21">
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
@@ -18877,7 +18877,7 @@
     <row r="5" spans="2:2">
       <c r="B5" s="42"/>
     </row>
-    <row r="6" spans="2:2" ht="60">
+    <row r="6" spans="2:2" ht="64">
       <c r="B6" s="267" t="s">
         <v>305</v>
       </c>
@@ -18927,7 +18927,7 @@
     <row r="18" spans="2:2">
       <c r="B18" s="42"/>
     </row>
-    <row r="19" spans="2:2" ht="90">
+    <row r="19" spans="2:2" ht="80">
       <c r="B19" s="124" t="s">
         <v>247</v>
       </c>
@@ -18958,9 +18958,9 @@
       <selection activeCell="CV35" sqref="CV35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.875" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="16384" width="2.83203125" style="1"/>
+    <col min="1" max="16384" width="2.875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:80" ht="20" customHeight="1">
@@ -19329,7 +19329,7 @@
       <c r="BU6" s="52"/>
       <c r="BV6" s="52"/>
     </row>
-    <row r="7" spans="2:80" ht="23">
+    <row r="7" spans="2:80" ht="25">
       <c r="B7" s="52"/>
       <c r="C7" s="64" t="s">
         <v>182</v>
@@ -19434,15 +19434,15 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.83203125" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="25.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="20">
+    <row r="2" spans="2:3" ht="21">
       <c r="B2" s="2" t="s">
         <v>23</v>
       </c>
@@ -19455,12 +19455,12 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:3" ht="75" customHeight="1">
-      <c r="B5" s="335" t="s">
+      <c r="B5" s="337" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="336"/>
-    </row>
-    <row r="6" spans="2:3" ht="16" thickBot="1"/>
+      <c r="C5" s="338"/>
+    </row>
+    <row r="6" spans="2:3" ht="17" thickBot="1"/>
     <row r="7" spans="2:3">
       <c r="B7" s="20" t="s">
         <v>28</v>
@@ -19485,13 +19485,13 @@
       </c>
       <c r="C10" s="27"/>
     </row>
-    <row r="11" spans="2:3" ht="30">
+    <row r="11" spans="2:3" ht="32">
       <c r="B11" s="22"/>
       <c r="C11" s="266" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="30">
+    <row r="12" spans="2:3" ht="32">
       <c r="B12" s="22"/>
       <c r="C12" s="266" t="s">
         <v>287</v>
@@ -19503,7 +19503,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="30">
+    <row r="14" spans="2:3" ht="32">
       <c r="B14" s="22"/>
       <c r="C14" s="266" t="s">
         <v>306</v>
@@ -19515,14 +19515,14 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="16" thickBot="1">
+    <row r="16" spans="2:3" ht="17" thickBot="1">
       <c r="B16" s="33"/>
       <c r="C16" s="65"/>
     </row>
     <row r="17" spans="2:3" s="8" customFormat="1">
       <c r="C17" s="45"/>
     </row>
-    <row r="18" spans="2:3" ht="16" thickBot="1">
+    <row r="18" spans="2:3" ht="17" thickBot="1">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
     </row>
@@ -19554,11 +19554,11 @@
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="16" thickBot="1">
+    <row r="24" spans="2:3" ht="17" thickBot="1">
       <c r="B24" s="85"/>
       <c r="C24" s="87"/>
     </row>
-    <row r="25" spans="2:3" ht="16" thickBot="1"/>
+    <row r="25" spans="2:3" ht="17" thickBot="1"/>
     <row r="26" spans="2:3">
       <c r="B26" s="20" t="s">
         <v>189</v>
@@ -19999,11 +19999,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="2:3" ht="16" thickBot="1">
+    <row r="99" spans="2:3" ht="17" thickBot="1">
       <c r="B99" s="33"/>
       <c r="C99" s="36"/>
     </row>
-    <row r="100" spans="2:3" ht="16" thickBot="1"/>
+    <row r="100" spans="2:3" ht="17" thickBot="1"/>
     <row r="101" spans="2:3">
       <c r="B101" s="20" t="s">
         <v>201</v>
@@ -20034,7 +20034,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="106" spans="2:3" ht="16" thickBot="1">
+    <row r="106" spans="2:3" ht="17" thickBot="1">
       <c r="B106" s="33"/>
       <c r="C106" s="47"/>
     </row>
@@ -20063,29 +20063,29 @@
   </sheetPr>
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="77.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="79.6640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="65.83203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="2.83203125" style="1" customWidth="1"/>
-    <col min="15" max="16" width="13.33203125" style="204" customWidth="1"/>
-    <col min="17" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="77.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="79.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="65.875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="2.875" style="1" customWidth="1"/>
+    <col min="15" max="16" width="13.375" style="204" customWidth="1"/>
+    <col min="17" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="20">
+    <row r="2" spans="1:16" ht="21">
       <c r="B2" s="2" t="s">
         <v>24</v>
       </c>
@@ -20095,7 +20095,7 @@
       <c r="J2" s="11"/>
       <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:16" ht="20">
+    <row r="3" spans="1:16" ht="21">
       <c r="B3" s="2"/>
       <c r="I3" s="209"/>
       <c r="J3" s="8"/>
@@ -20114,38 +20114,38 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="B5" s="337" t="s">
+      <c r="B5" s="339" t="s">
         <v>307</v>
       </c>
-      <c r="C5" s="338"/>
-      <c r="D5" s="338"/>
-      <c r="E5" s="339"/>
+      <c r="C5" s="340"/>
+      <c r="D5" s="340"/>
+      <c r="E5" s="341"/>
       <c r="F5" s="8"/>
       <c r="I5" s="229"/>
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="B6" s="337"/>
-      <c r="C6" s="338"/>
-      <c r="D6" s="338"/>
-      <c r="E6" s="339"/>
+      <c r="B6" s="339"/>
+      <c r="C6" s="340"/>
+      <c r="D6" s="340"/>
+      <c r="E6" s="341"/>
       <c r="F6" s="8"/>
       <c r="I6" s="207"/>
       <c r="J6" s="8"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="B7" s="335"/>
-      <c r="C7" s="340"/>
-      <c r="D7" s="340"/>
-      <c r="E7" s="336"/>
+      <c r="B7" s="337"/>
+      <c r="C7" s="342"/>
+      <c r="D7" s="342"/>
+      <c r="E7" s="338"/>
       <c r="F7" s="151"/>
       <c r="I7" s="228"/>
       <c r="J7" s="9"/>
       <c r="K7" s="10"/>
     </row>
-    <row r="8" spans="1:16" ht="16" thickBot="1"/>
+    <row r="8" spans="1:16" ht="17" thickBot="1"/>
     <row r="9" spans="1:16">
       <c r="B9" s="20" t="s">
         <v>23</v>
@@ -20848,7 +20848,7 @@
       <c r="O36" s="207"/>
       <c r="P36" s="208"/>
     </row>
-    <row r="37" spans="1:16" ht="16" thickBot="1">
+    <row r="37" spans="1:16" ht="17" thickBot="1">
       <c r="A37" s="8"/>
       <c r="B37" s="28"/>
       <c r="C37" s="12"/>
@@ -20866,11 +20866,11 @@
       <c r="O37" s="207"/>
       <c r="P37" s="208"/>
     </row>
-    <row r="38" spans="1:16" ht="16" thickBot="1">
+    <row r="38" spans="1:16" ht="17" thickBot="1">
       <c r="A38" s="8"/>
       <c r="B38" s="28"/>
       <c r="C38" s="162" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D38" s="157"/>
       <c r="E38" s="291"/>
@@ -20932,7 +20932,7 @@
       <c r="O40" s="207"/>
       <c r="P40" s="208"/>
     </row>
-    <row r="41" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="41" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A41" s="8"/>
       <c r="B41" s="22" t="s">
         <v>283</v>
@@ -20952,7 +20952,7 @@
       <c r="O41" s="207"/>
       <c r="P41" s="208"/>
     </row>
-    <row r="42" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="42" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A42" s="8"/>
       <c r="B42" s="22"/>
       <c r="C42" s="258" t="s">
@@ -20987,7 +20987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="43" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A43" s="8"/>
       <c r="B43" s="22"/>
       <c r="C43" s="258" t="s">
@@ -21022,7 +21022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="44" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A44" s="8"/>
       <c r="B44" s="22"/>
       <c r="C44" s="258" t="s">
@@ -21057,7 +21057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="45" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A45" s="8"/>
       <c r="B45" s="22"/>
       <c r="C45" s="258" t="s">
@@ -21092,7 +21092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="46" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A46" s="8"/>
       <c r="B46" s="22"/>
       <c r="C46" s="258" t="s">
@@ -21127,7 +21127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="47" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A47" s="8"/>
       <c r="B47" s="22"/>
       <c r="C47" s="258" t="s">
@@ -21180,7 +21180,7 @@
       <c r="O48" s="207"/>
       <c r="P48" s="7"/>
     </row>
-    <row r="49" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="49" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A49" s="8"/>
       <c r="B49" s="22" t="s">
         <v>284</v>
@@ -21200,7 +21200,7 @@
       <c r="O49" s="207"/>
       <c r="P49" s="208"/>
     </row>
-    <row r="50" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="50" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A50" s="8"/>
       <c r="B50" s="22"/>
       <c r="C50" s="258" t="s">
@@ -21235,7 +21235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="51" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A51" s="8"/>
       <c r="B51" s="22"/>
       <c r="C51" s="258" t="s">
@@ -21270,7 +21270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="16" outlineLevel="1" thickBot="1">
+    <row r="52" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
       <c r="A52" s="8"/>
       <c r="B52" s="22"/>
       <c r="C52" s="258" t="s">
@@ -21305,7 +21305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="16" thickBot="1">
+    <row r="53" spans="1:16" ht="17" thickBot="1">
       <c r="B53" s="33"/>
       <c r="C53" s="46"/>
       <c r="D53" s="159"/>
@@ -21508,15 +21508,15 @@
       <selection pane="bottomRight" activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="50.83203125" style="1" customWidth="1"/>
-    <col min="3" max="67" width="13.6640625" style="1" customWidth="1"/>
-    <col min="68" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="50.875" style="1" customWidth="1"/>
+    <col min="3" max="67" width="13.625" style="1" customWidth="1"/>
+    <col min="68" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:67" ht="20">
+    <row r="2" spans="2:67" ht="21">
       <c r="B2" s="2" t="s">
         <v>265</v>
       </c>
@@ -21529,7 +21529,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30">
+    <row r="5" spans="2:67" ht="32">
       <c r="B5" s="125" t="s">
         <v>256</v>
       </c>
@@ -22155,7 +22155,7 @@
       <c r="BN13" s="183"/>
       <c r="BO13" s="184"/>
     </row>
-    <row r="14" spans="2:67" ht="16" thickBot="1">
+    <row r="14" spans="2:67" ht="17" thickBot="1">
       <c r="B14" s="181" t="s">
         <v>112</v>
       </c>
@@ -22225,7 +22225,7 @@
       <c r="BN14" s="183"/>
       <c r="BO14" s="184"/>
     </row>
-    <row r="15" spans="2:67" ht="16" thickBot="1">
+    <row r="15" spans="2:67" ht="17" thickBot="1">
       <c r="B15" s="185" t="s">
         <v>113</v>
       </c>
@@ -22365,7 +22365,7 @@
       <c r="BN16" s="183"/>
       <c r="BO16" s="184"/>
     </row>
-    <row r="17" spans="2:67" ht="16" thickBot="1">
+    <row r="17" spans="2:67" ht="17" thickBot="1">
       <c r="B17" s="181" t="s">
         <v>115</v>
       </c>
@@ -22435,7 +22435,7 @@
       <c r="BN17" s="183"/>
       <c r="BO17" s="184"/>
     </row>
-    <row r="18" spans="2:67" ht="16" thickBot="1">
+    <row r="18" spans="2:67" ht="17" thickBot="1">
       <c r="B18" s="185" t="s">
         <v>116</v>
       </c>
@@ -23905,7 +23905,7 @@
       <c r="BN38" s="183"/>
       <c r="BO38" s="184"/>
     </row>
-    <row r="39" spans="2:67" ht="16" thickBot="1">
+    <row r="39" spans="2:67" ht="17" thickBot="1">
       <c r="B39" s="181" t="s">
         <v>129</v>
       </c>
@@ -23975,7 +23975,7 @@
       <c r="BN39" s="183"/>
       <c r="BO39" s="184"/>
     </row>
-    <row r="40" spans="2:67" ht="16" thickBot="1">
+    <row r="40" spans="2:67" ht="17" thickBot="1">
       <c r="B40" s="185" t="s">
         <v>130</v>
       </c>
@@ -25235,7 +25235,7 @@
       <c r="BN57" s="183"/>
       <c r="BO57" s="184"/>
     </row>
-    <row r="58" spans="2:67" ht="16" thickBot="1">
+    <row r="58" spans="2:67" ht="17" thickBot="1">
       <c r="B58" s="181" t="s">
         <v>139</v>
       </c>
@@ -25305,7 +25305,7 @@
       <c r="BN58" s="183"/>
       <c r="BO58" s="184"/>
     </row>
-    <row r="59" spans="2:67" ht="16" thickBot="1">
+    <row r="59" spans="2:67" ht="17" thickBot="1">
       <c r="B59" s="185" t="s">
         <v>140</v>
       </c>
@@ -25375,7 +25375,7 @@
       <c r="BN59" s="187"/>
       <c r="BO59" s="188"/>
     </row>
-    <row r="60" spans="2:67" ht="16" thickBot="1">
+    <row r="60" spans="2:67" ht="17" thickBot="1">
       <c r="B60" s="185" t="s">
         <v>25</v>
       </c>
@@ -26285,7 +26285,7 @@
       <c r="BN72" s="183"/>
       <c r="BO72" s="184"/>
     </row>
-    <row r="73" spans="2:67" ht="16" thickBot="1">
+    <row r="73" spans="2:67" ht="17" thickBot="1">
       <c r="B73" s="181" t="s">
         <v>153</v>
       </c>
@@ -26355,7 +26355,7 @@
       <c r="BN73" s="183"/>
       <c r="BO73" s="184"/>
     </row>
-    <row r="74" spans="2:67" ht="16" thickBot="1">
+    <row r="74" spans="2:67" ht="17" thickBot="1">
       <c r="B74" s="185" t="s">
         <v>154</v>
       </c>
@@ -26775,7 +26775,7 @@
       <c r="BN79" s="183"/>
       <c r="BO79" s="184"/>
     </row>
-    <row r="80" spans="2:67" ht="16" thickBot="1">
+    <row r="80" spans="2:67" ht="17" thickBot="1">
       <c r="B80" s="181" t="s">
         <v>160</v>
       </c>
@@ -26845,7 +26845,7 @@
       <c r="BN80" s="183"/>
       <c r="BO80" s="184"/>
     </row>
-    <row r="81" spans="2:67" ht="16" thickBot="1">
+    <row r="81" spans="2:67" ht="17" thickBot="1">
       <c r="B81" s="185" t="s">
         <v>82</v>
       </c>
@@ -27195,7 +27195,7 @@
       <c r="BN85" s="183"/>
       <c r="BO85" s="184"/>
     </row>
-    <row r="86" spans="2:67" ht="16" thickBot="1">
+    <row r="86" spans="2:67" ht="17" thickBot="1">
       <c r="B86" s="181" t="s">
         <v>165</v>
       </c>
@@ -27265,7 +27265,7 @@
       <c r="BN86" s="183"/>
       <c r="BO86" s="184"/>
     </row>
-    <row r="87" spans="2:67" ht="16" thickBot="1">
+    <row r="87" spans="2:67" ht="17" thickBot="1">
       <c r="B87" s="185" t="s">
         <v>166</v>
       </c>
@@ -27545,7 +27545,7 @@
       <c r="BN90" s="183"/>
       <c r="BO90" s="184"/>
     </row>
-    <row r="91" spans="2:67" ht="16" thickBot="1">
+    <row r="91" spans="2:67" ht="17" thickBot="1">
       <c r="B91" s="181" t="s">
         <v>170</v>
       </c>
@@ -27615,7 +27615,7 @@
       <c r="BN91" s="183"/>
       <c r="BO91" s="184"/>
     </row>
-    <row r="92" spans="2:67" ht="16" thickBot="1">
+    <row r="92" spans="2:67" ht="17" thickBot="1">
       <c r="B92" s="185" t="s">
         <v>171</v>
       </c>
@@ -27895,7 +27895,7 @@
       <c r="BN95" s="183"/>
       <c r="BO95" s="184"/>
     </row>
-    <row r="96" spans="2:67" ht="16" thickBot="1">
+    <row r="96" spans="2:67" ht="17" thickBot="1">
       <c r="B96" s="181" t="s">
         <v>175</v>
       </c>
@@ -27965,7 +27965,7 @@
       <c r="BN96" s="183"/>
       <c r="BO96" s="184"/>
     </row>
-    <row r="97" spans="2:67" ht="16" thickBot="1">
+    <row r="97" spans="2:67" ht="17" thickBot="1">
       <c r="B97" s="185" t="s">
         <v>176</v>
       </c>
@@ -28245,7 +28245,7 @@
       <c r="BN100" s="183"/>
       <c r="BO100" s="184"/>
     </row>
-    <row r="101" spans="2:67" ht="16" thickBot="1">
+    <row r="101" spans="2:67" ht="17" thickBot="1">
       <c r="B101" s="196" t="s">
         <v>180</v>
       </c>
@@ -28338,22 +28338,22 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.1640625" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="19" width="14.1640625" style="1" customWidth="1"/>
-    <col min="20" max="21" width="20.83203125" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="2" max="2" width="21.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.125" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="52.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="19" width="14.125" style="1" customWidth="1"/>
+    <col min="20" max="21" width="20.875" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
       <c r="E1" s="90"/>
     </row>
-    <row r="2" spans="2:13" ht="20">
+    <row r="2" spans="2:13" ht="21">
       <c r="B2" s="81" t="s">
         <v>203</v>
       </c>
@@ -28380,11 +28380,11 @@
       <c r="M4" s="8"/>
     </row>
     <row r="5" spans="2:13" ht="60" customHeight="1">
-      <c r="B5" s="341" t="s">
+      <c r="B5" s="343" t="s">
         <v>300</v>
       </c>
-      <c r="C5" s="342"/>
-      <c r="D5" s="342"/>
+      <c r="C5" s="344"/>
+      <c r="D5" s="344"/>
       <c r="E5" s="272"/>
       <c r="F5" s="45"/>
       <c r="G5" s="45"/>
@@ -28395,7 +28395,7 @@
       <c r="L5" s="45"/>
       <c r="M5" s="45"/>
     </row>
-    <row r="6" spans="2:13" ht="16" thickBot="1">
+    <row r="6" spans="2:13" ht="17" thickBot="1">
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
@@ -28517,7 +28517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="16" thickBot="1">
+    <row r="16" spans="2:13" ht="17" thickBot="1">
       <c r="B16" s="85"/>
       <c r="C16" s="86"/>
       <c r="D16" s="86"/>

</xml_diff>

<commit_message>
published state of ETdataset on 7th of February 2020 -2
</commit_message>
<xml_diff>
--- a/analyses/4b_chemical_industry_analysis.xlsx
+++ b/analyses/4b_chemical_industry_analysis.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28421"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10113"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/analyses/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74357124-6874-504C-9979-96F2F0D60997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="835" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38200" windowHeight="25720" tabRatio="835" firstSheet="11" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -42,6 +48,7 @@
   <externalReferences>
     <externalReference r:id="rId32"/>
     <externalReference r:id="rId33"/>
+    <externalReference r:id="rId34"/>
   </externalReferences>
   <definedNames>
     <definedName name="aluminium_production" localSheetId="18">Dashboard!#REF!</definedName>
@@ -663,31 +670,38 @@
     <definedName name="steel_production" localSheetId="16">Dashboard!#REF!</definedName>
     <definedName name="steel_production">Dashboard!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentManualCount="4"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>A satisfied Microsoft Office user</author>
   </authors>
   <commentList>
-    <comment ref="U83" authorId="0">
+    <comment ref="U83" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0700-000001000000}">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">x  Not Applicable
 </t>
@@ -699,7 +713,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="786" uniqueCount="480">
   <si>
     <t>Changelog</t>
   </si>
@@ -2136,20 +2150,23 @@
   </si>
   <si>
     <t>Electricity consumption for heat pumps</t>
+  </si>
+  <si>
+    <t>nl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
-    <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="168" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2198,6 +2215,7 @@
       <sz val="16"/>
       <color theme="3"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2213,11 +2231,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2225,6 +2245,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2238,6 +2259,7 @@
       <u/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2267,6 +2289,7 @@
       <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2274,12 +2297,14 @@
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -2292,6 +2317,7 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2299,17 +2325,20 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2317,12 +2346,14 @@
       <sz val="12"/>
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2330,6 +2361,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -5072,7 +5104,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5196,11 +5228,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5230,7 +5262,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5243,36 +5275,36 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -5287,7 +5319,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5310,44 +5342,44 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5366,10 +5398,10 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5443,8 +5475,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -5464,10 +5496,10 @@
     <xf numFmtId="0" fontId="24" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5476,18 +5508,18 @@
     <xf numFmtId="3" fontId="9" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5535,10 +5567,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5625,7 +5657,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5655,21 +5687,21 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="5" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -5689,13 +5721,13 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5704,38 +5736,38 @@
     <xf numFmtId="3" fontId="9" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -5763,8 +5795,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="2061" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -5807,8 +5841,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="2061" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="1" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2074">
     <cellStyle name="Comma" xfId="2061" builtinId="3"/>
@@ -7883,8 +7915,8 @@
     <cellStyle name="Hyperlink" xfId="2070" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2072" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="772"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent 2" xfId="772" xr:uid="{00000000-0005-0000-0000-000019080000}"/>
   </cellStyles>
   <dxfs count="30">
     <dxf>
@@ -8229,6 +8261,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -8262,7 +8297,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="157" name="Rectangle 156"/>
+        <xdr:cNvPr id="157" name="Rectangle 156">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00009D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8329,7 +8370,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="93" name="L-Shape 92"/>
+        <xdr:cNvPr id="93" name="L-Shape 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8393,7 +8440,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="104" name="Rectangle 103"/>
+        <xdr:cNvPr id="104" name="Rectangle 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000068000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8546,7 +8599,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 1"/>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8609,7 +8668,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="Rectangle 2"/>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8672,7 +8737,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4"/>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8735,7 +8806,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Rectangle 5"/>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8796,7 +8873,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Rectangle 6"/>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8857,7 +8940,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="Rectangle 7"/>
+        <xdr:cNvPr id="8" name="Rectangle 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -8932,7 +9021,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Straight Connector 8"/>
+        <xdr:cNvPr id="9" name="Straight Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -8982,7 +9077,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="11" name="Straight Connector 10"/>
+        <xdr:cNvPr id="11" name="Straight Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00000B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -9032,7 +9133,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="Straight Connector 17"/>
+        <xdr:cNvPr id="18" name="Straight Connector 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000012000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -9082,7 +9189,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="Rectangle 30"/>
+        <xdr:cNvPr id="31" name="Rectangle 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00001F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9143,7 +9256,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="Rectangle 38"/>
+        <xdr:cNvPr id="39" name="Rectangle 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000027000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9204,7 +9323,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="149" name="Rectangle 148"/>
+        <xdr:cNvPr id="149" name="Rectangle 148">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000095000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9260,7 +9385,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="181" name="Rectangle 180"/>
+        <xdr:cNvPr id="181" name="Rectangle 180">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-0000B5000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9321,7 +9452,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="358" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="358" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000066010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="181" idx="3"/>
           <a:endCxn id="363" idx="1"/>
@@ -9371,7 +9508,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="363" name="Rectangle 362"/>
+        <xdr:cNvPr id="363" name="Rectangle 362">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00006B010000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9431,7 +9574,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="136" name="Rectangle 135"/>
+        <xdr:cNvPr id="136" name="Rectangle 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000088000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9487,7 +9636,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="100" name="Rectangle 99"/>
+        <xdr:cNvPr id="100" name="Rectangle 99">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000064000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9546,7 +9701,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="102" name="Rectangle 101"/>
+        <xdr:cNvPr id="102" name="Rectangle 101">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000066000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9605,7 +9766,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="50" name="Straight Arrow Connector 49"/>
+        <xdr:cNvPr id="50" name="Straight Arrow Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000032000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="3" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -9654,7 +9821,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="114" name="Straight Arrow Connector 113"/>
+        <xdr:cNvPr id="114" name="Straight Arrow Connector 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000072000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="2" idx="2"/>
         </xdr:cNvCxnSpPr>
@@ -9703,7 +9876,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="92" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="92" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="7" idx="3"/>
           <a:endCxn id="39" idx="1"/>
@@ -9753,7 +9932,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="95" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="95" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00005F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="39" idx="3"/>
           <a:endCxn id="149" idx="1"/>
@@ -9803,7 +9988,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="103" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="103" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000067000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="149" idx="3"/>
           <a:endCxn id="181" idx="1"/>
@@ -9853,7 +10044,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="Rectangle 41"/>
+        <xdr:cNvPr id="42" name="Rectangle 41">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002A000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -9914,7 +10111,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="43" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="43" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="42" idx="3"/>
         </xdr:cNvCxnSpPr>
@@ -9963,7 +10166,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="Rectangle 43"/>
+        <xdr:cNvPr id="44" name="Rectangle 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002C000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10019,7 +10228,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="45" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="45" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002D000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10066,7 +10281,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="Rectangle 45"/>
+        <xdr:cNvPr id="46" name="Rectangle 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002E000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10122,7 +10343,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="47" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="47" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00002F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="181" idx="2"/>
           <a:endCxn id="42" idx="0"/>
@@ -10172,7 +10399,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="64" name="Straight Connector 63"/>
+        <xdr:cNvPr id="64" name="Straight Connector 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000040000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10216,7 +10449,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="66" name="Straight Connector 65"/>
+        <xdr:cNvPr id="66" name="Straight Connector 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000042000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10260,7 +10499,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="69" name="Straight Connector 68"/>
+        <xdr:cNvPr id="69" name="Straight Connector 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000045000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10304,7 +10549,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="37" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000025000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="7" idx="3"/>
           <a:endCxn id="40" idx="1"/>
@@ -10356,7 +10607,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="Rectangle 39"/>
+        <xdr:cNvPr id="40" name="Rectangle 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000028000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10412,7 +10669,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="48" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000030000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="149" idx="2"/>
           <a:endCxn id="49" idx="0"/>
@@ -10462,7 +10725,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="Rectangle 48"/>
+        <xdr:cNvPr id="49" name="Rectangle 48">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000031000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10518,7 +10787,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="51" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="51" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000033000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="40" idx="3"/>
           <a:endCxn id="54" idx="1"/>
@@ -10570,7 +10845,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="Rectangle 53"/>
+        <xdr:cNvPr id="54" name="Rectangle 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000036000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10626,7 +10907,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="55" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="55" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000037000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -10673,7 +10960,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="56" name="Rectangle 55"/>
+        <xdr:cNvPr id="56" name="Rectangle 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000038000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -10729,7 +11022,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="59" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="59" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003B000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="49" idx="2"/>
           <a:endCxn id="54" idx="1"/>
@@ -10779,7 +11078,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="63" name="Elbow Connector 195"/>
+        <xdr:cNvPr id="63" name="Elbow Connector 195">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-00003F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="31" idx="3"/>
           <a:endCxn id="49" idx="1"/>
@@ -10841,11 +11146,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s11265"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-0000012C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -10853,6 +11161,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -10862,13 +11176,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>import data</a:t>
               </a:r>
@@ -10902,11 +11215,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s11266"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-0000022C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -10914,6 +11230,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -10923,13 +11245,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>export to 'data/…/ouput' folder</a:t>
               </a:r>
@@ -10963,11 +11284,14 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s11272"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-0000082C0000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr>
+          <xdr:spPr bwMode="auto">
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -10975,6 +11299,12 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
           </xdr:spPr>
           <xdr:txBody>
             <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
@@ -10984,13 +11314,12 @@
                 <a:defRPr sz="1000"/>
               </a:pPr>
               <a:r>
-                <a:rPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                <a:rPr lang="en-GB" sz="1200" b="0" i="0" u="none" strike="noStrike" baseline="0">
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Lucida Grande"/>
-                  <a:ea typeface="Lucida Grande"/>
-                  <a:cs typeface="Lucida Grande"/>
+                  <a:latin typeface="Lucida Grande" pitchFamily="2" charset="0"/>
+                  <a:cs typeface="Lucida Grande" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>optional: load dashboard values</a:t>
               </a:r>
@@ -11012,7 +11341,13 @@
     <xdr:ext cx="7152619" cy="276999"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="TextBox 5"/>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -11063,7 +11398,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover Sheet"/>
@@ -11420,12 +11755,13 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Cover sheet"/>
       <sheetName val="Dashboard"/>
       <sheetName val="analysis_manager.xlsm"/>
+      <sheetName val="analysis_manager"/>
     </sheetNames>
     <definedNames>
       <definedName name="export_data_button"/>
@@ -11436,6 +11772,27 @@
       <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1" refreshError="1"/>
       <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover sheet"/>
+      <sheetName val="Dashboard"/>
+    </sheetNames>
+    <definedNames>
+      <definedName name="export_data_button"/>
+      <definedName name="import_data_button"/>
+      <definedName name="select_dashboard_values"/>
+    </definedNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -11762,8 +12119,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Sheet1">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:D38"/>
@@ -11772,13 +12129,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="13.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="44" style="1" customWidth="1"/>
-    <col min="4" max="7" width="10.875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.625" style="1"/>
+    <col min="4" max="7" width="10.83203125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="21">
@@ -11809,9 +12166,9 @@
       <c r="B6" s="281" t="s">
         <v>205</v>
       </c>
-      <c r="C6" s="94">
+      <c r="C6" s="94" t="str">
         <f>country</f>
-        <v>0</v>
+        <v>nl</v>
       </c>
       <c r="D6" s="7"/>
     </row>
@@ -11821,7 +12178,7 @@
       </c>
       <c r="C7" s="94">
         <f>base_year</f>
-        <v>0</v>
+        <v>2015</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -12034,8 +12391,8 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet10" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr codeName="Sheet10">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:Q36"/>
@@ -12044,14 +12401,14 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
     <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" style="90" customWidth="1"/>
-    <col min="6" max="10" width="14.375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="1"/>
+    <col min="3" max="4" width="14.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="90" customWidth="1"/>
+    <col min="6" max="10" width="14.33203125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -12117,12 +12474,12 @@
     </row>
     <row r="5" spans="1:17" ht="113" customHeight="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="358" t="s">
+      <c r="B5" s="360" t="s">
         <v>450</v>
       </c>
-      <c r="C5" s="359"/>
-      <c r="D5" s="359"/>
-      <c r="E5" s="360"/>
+      <c r="C5" s="361"/>
+      <c r="D5" s="361"/>
+      <c r="E5" s="362"/>
       <c r="F5" s="82"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
@@ -12180,7 +12537,7 @@
       <c r="M8" s="82"/>
       <c r="N8" s="82"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" ht="34">
       <c r="A9" s="82"/>
       <c r="B9" s="115"/>
       <c r="C9" s="155" t="s">
@@ -12217,7 +12574,7 @@
       <c r="P9" s="82"/>
       <c r="Q9" s="82"/>
     </row>
-    <row r="10" spans="1:17" ht="32">
+    <row r="10" spans="1:17" ht="34">
       <c r="A10" s="82"/>
       <c r="B10" s="106" t="s">
         <v>402</v>
@@ -12264,7 +12621,7 @@
       <c r="P10" s="82"/>
       <c r="Q10" s="82"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" ht="17">
       <c r="A11" s="82"/>
       <c r="B11" s="105" t="s">
         <v>309</v>
@@ -12311,7 +12668,7 @@
       <c r="P11" s="82"/>
       <c r="Q11" s="82"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" ht="17">
       <c r="A12" s="82"/>
       <c r="B12" s="251" t="s">
         <v>310</v>
@@ -12358,7 +12715,7 @@
       <c r="P12" s="82"/>
       <c r="Q12" s="82"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" ht="17">
       <c r="A13" s="82"/>
       <c r="B13" s="251" t="s">
         <v>82</v>
@@ -12424,7 +12781,7 @@
       <c r="P14" s="82"/>
       <c r="Q14" s="82"/>
     </row>
-    <row r="15" spans="1:17" ht="32">
+    <row r="15" spans="1:17" ht="34">
       <c r="A15" s="82"/>
       <c r="B15" s="106" t="s">
         <v>403</v>
@@ -12472,7 +12829,7 @@
       <c r="P15" s="82"/>
       <c r="Q15" s="82"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" ht="17">
       <c r="A16" s="82"/>
       <c r="B16" s="251" t="s">
         <v>309</v>
@@ -12519,7 +12876,7 @@
       <c r="P16" s="82"/>
       <c r="Q16" s="82"/>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" ht="17">
       <c r="A17" s="82"/>
       <c r="B17" s="251" t="s">
         <v>310</v>
@@ -12566,7 +12923,7 @@
       <c r="P17" s="82"/>
       <c r="Q17" s="82"/>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" ht="17">
       <c r="A18" s="82"/>
       <c r="B18" s="251" t="s">
         <v>82</v>
@@ -12934,8 +13291,8 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet11" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr codeName="Sheet11">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:Q61"/>
@@ -12944,15 +13301,15 @@
       <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="3" width="21.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="90" customWidth="1"/>
-    <col min="7" max="11" width="14.375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="3" width="21.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="90" customWidth="1"/>
+    <col min="7" max="11" width="14.33203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -13021,13 +13378,13 @@
     </row>
     <row r="5" spans="1:14" ht="41" customHeight="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="358" t="s">
+      <c r="B5" s="360" t="s">
         <v>335</v>
       </c>
-      <c r="C5" s="359"/>
-      <c r="D5" s="359"/>
-      <c r="E5" s="359"/>
-      <c r="F5" s="360"/>
+      <c r="C5" s="361"/>
+      <c r="D5" s="361"/>
+      <c r="E5" s="361"/>
+      <c r="F5" s="362"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
       <c r="I5" s="82"/>
@@ -13074,7 +13431,7 @@
       <c r="G8" s="82"/>
       <c r="H8" s="82"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="17">
       <c r="A9" s="82"/>
       <c r="B9" s="132" t="s">
         <v>333</v>
@@ -13095,7 +13452,7 @@
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="17">
       <c r="A10" s="82"/>
       <c r="B10" s="135" t="s">
         <v>190</v>
@@ -13110,7 +13467,7 @@
       <c r="J10" s="82"/>
       <c r="K10" s="82"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="17">
       <c r="A11" s="82"/>
       <c r="B11" s="134"/>
       <c r="C11" s="143" t="s">
@@ -13131,7 +13488,7 @@
       <c r="J11" s="82"/>
       <c r="K11" s="82"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="17">
       <c r="A12" s="82"/>
       <c r="B12" s="251"/>
       <c r="C12" s="303" t="s">
@@ -13152,7 +13509,7 @@
       <c r="J12" s="82"/>
       <c r="K12" s="82"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="17">
       <c r="A13" s="82"/>
       <c r="B13" s="251"/>
       <c r="C13" s="303" t="s">
@@ -13186,7 +13543,7 @@
       <c r="J14" s="82"/>
       <c r="K14" s="82"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="17">
       <c r="A15" s="82"/>
       <c r="B15" s="304" t="s">
         <v>209</v>
@@ -13201,7 +13558,7 @@
       <c r="J15" s="82"/>
       <c r="K15" s="82"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="17">
       <c r="A16" s="82"/>
       <c r="B16" s="251"/>
       <c r="C16" s="303" t="s">
@@ -13222,7 +13579,7 @@
       <c r="J16" s="82"/>
       <c r="K16" s="82"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="17">
       <c r="A17" s="82"/>
       <c r="B17" s="251"/>
       <c r="C17" s="303" t="s">
@@ -13243,7 +13600,7 @@
       <c r="J17" s="82"/>
       <c r="K17" s="82"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="17">
       <c r="A18" s="82"/>
       <c r="B18" s="251"/>
       <c r="C18" s="303" t="s">
@@ -13277,7 +13634,7 @@
       <c r="J19" s="82"/>
       <c r="K19" s="82"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="17">
       <c r="A20" s="82"/>
       <c r="B20" s="304" t="s">
         <v>51</v>
@@ -13292,7 +13649,7 @@
       <c r="J20" s="82"/>
       <c r="K20" s="82"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="17">
       <c r="A21" s="82"/>
       <c r="B21" s="251"/>
       <c r="C21" s="303" t="s">
@@ -13313,7 +13670,7 @@
       <c r="J21" s="82"/>
       <c r="K21" s="82"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" ht="17">
       <c r="A22" s="82"/>
       <c r="B22" s="251"/>
       <c r="C22" s="303" t="s">
@@ -13334,7 +13691,7 @@
       <c r="J22" s="82"/>
       <c r="K22" s="82"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="17">
       <c r="A23" s="82"/>
       <c r="B23" s="251"/>
       <c r="C23" s="303" t="s">
@@ -13368,7 +13725,7 @@
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="17">
       <c r="A25" s="82"/>
       <c r="B25" s="304" t="s">
         <v>192</v>
@@ -13383,7 +13740,7 @@
       <c r="J25" s="82"/>
       <c r="K25" s="82"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="17">
       <c r="A26" s="82"/>
       <c r="B26" s="251"/>
       <c r="C26" s="303" t="s">
@@ -13404,7 +13761,7 @@
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="17">
       <c r="A27" s="82"/>
       <c r="B27" s="251"/>
       <c r="C27" s="303" t="s">
@@ -13425,7 +13782,7 @@
       <c r="J27" s="82"/>
       <c r="K27" s="82"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" ht="17">
       <c r="A28" s="82"/>
       <c r="B28" s="251"/>
       <c r="C28" s="303" t="s">
@@ -13459,7 +13816,7 @@
       <c r="J29" s="82"/>
       <c r="K29" s="82"/>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" ht="17">
       <c r="A30" s="82"/>
       <c r="B30" s="304" t="s">
         <v>104</v>
@@ -13474,7 +13831,7 @@
       <c r="J30" s="82"/>
       <c r="K30" s="82"/>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" ht="17">
       <c r="A31" s="82"/>
       <c r="B31" s="251"/>
       <c r="C31" s="303" t="s">
@@ -13495,7 +13852,7 @@
       <c r="J31" s="82"/>
       <c r="K31" s="82"/>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" ht="17">
       <c r="A32" s="82"/>
       <c r="B32" s="251"/>
       <c r="C32" s="303" t="s">
@@ -13516,7 +13873,7 @@
       <c r="J32" s="82"/>
       <c r="K32" s="82"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" ht="17">
       <c r="A33" s="82"/>
       <c r="B33" s="251"/>
       <c r="C33" s="303" t="s">
@@ -13550,7 +13907,7 @@
       <c r="J34" s="82"/>
       <c r="K34" s="82"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" ht="17">
       <c r="A35" s="82"/>
       <c r="B35" s="304" t="s">
         <v>103</v>
@@ -13565,7 +13922,7 @@
       <c r="J35" s="82"/>
       <c r="K35" s="82"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" ht="17">
       <c r="A36" s="82"/>
       <c r="B36" s="251"/>
       <c r="C36" s="303" t="s">
@@ -13586,7 +13943,7 @@
       <c r="J36" s="82"/>
       <c r="K36" s="82"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" ht="17">
       <c r="A37" s="82"/>
       <c r="B37" s="251"/>
       <c r="C37" s="303" t="s">
@@ -13607,7 +13964,7 @@
       <c r="J37" s="82"/>
       <c r="K37" s="82"/>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" ht="17">
       <c r="A38" s="82"/>
       <c r="B38" s="251"/>
       <c r="C38" s="303" t="s">
@@ -13641,7 +13998,7 @@
       <c r="J39" s="82"/>
       <c r="K39" s="82"/>
     </row>
-    <row r="40" spans="1:17" ht="32">
+    <row r="40" spans="1:17" ht="34">
       <c r="A40" s="82"/>
       <c r="B40" s="304" t="s">
         <v>338</v>
@@ -13656,7 +14013,7 @@
       <c r="J40" s="82"/>
       <c r="K40" s="82"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" ht="17">
       <c r="A41" s="82"/>
       <c r="B41" s="251"/>
       <c r="C41" s="303" t="s">
@@ -13677,7 +14034,7 @@
       <c r="J41" s="82"/>
       <c r="K41" s="82"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" ht="17">
       <c r="A42" s="82"/>
       <c r="B42" s="251"/>
       <c r="C42" s="303" t="s">
@@ -13698,7 +14055,7 @@
       <c r="J42" s="82"/>
       <c r="K42" s="82"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" ht="17">
       <c r="A43" s="82"/>
       <c r="B43" s="251"/>
       <c r="C43" s="303" t="s">
@@ -14045,8 +14402,8 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr codeName="Sheet12">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:Q61"/>
@@ -14055,15 +14412,15 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="3" width="21.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="22.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.375" style="90" customWidth="1"/>
-    <col min="7" max="11" width="14.375" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="3" width="21.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" style="90" customWidth="1"/>
+    <col min="7" max="11" width="14.33203125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -14132,13 +14489,13 @@
     </row>
     <row r="5" spans="1:14" ht="41" customHeight="1">
       <c r="A5" s="82"/>
-      <c r="B5" s="358" t="s">
+      <c r="B5" s="360" t="s">
         <v>339</v>
       </c>
-      <c r="C5" s="359"/>
-      <c r="D5" s="359"/>
-      <c r="E5" s="359"/>
-      <c r="F5" s="360"/>
+      <c r="C5" s="361"/>
+      <c r="D5" s="361"/>
+      <c r="E5" s="361"/>
+      <c r="F5" s="362"/>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
       <c r="I5" s="82"/>
@@ -14185,7 +14542,7 @@
       <c r="G8" s="82"/>
       <c r="H8" s="82"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" ht="17">
       <c r="A9" s="82"/>
       <c r="B9" s="132" t="s">
         <v>333</v>
@@ -14206,7 +14563,7 @@
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" ht="17">
       <c r="A10" s="82"/>
       <c r="B10" s="135" t="s">
         <v>190</v>
@@ -14221,7 +14578,7 @@
       <c r="J10" s="82"/>
       <c r="K10" s="82"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" ht="17">
       <c r="A11" s="82"/>
       <c r="B11" s="134"/>
       <c r="C11" s="143" t="s">
@@ -14242,7 +14599,7 @@
       <c r="J11" s="82"/>
       <c r="K11" s="82"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" ht="17">
       <c r="A12" s="82"/>
       <c r="B12" s="251"/>
       <c r="C12" s="303" t="s">
@@ -14263,7 +14620,7 @@
       <c r="J12" s="82"/>
       <c r="K12" s="82"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" ht="17">
       <c r="A13" s="82"/>
       <c r="B13" s="251"/>
       <c r="C13" s="303" t="s">
@@ -14297,7 +14654,7 @@
       <c r="J14" s="82"/>
       <c r="K14" s="82"/>
     </row>
-    <row r="15" spans="1:14">
+    <row r="15" spans="1:14" ht="17">
       <c r="A15" s="82"/>
       <c r="B15" s="304" t="s">
         <v>209</v>
@@ -14312,7 +14669,7 @@
       <c r="J15" s="82"/>
       <c r="K15" s="82"/>
     </row>
-    <row r="16" spans="1:14">
+    <row r="16" spans="1:14" ht="17">
       <c r="A16" s="82"/>
       <c r="B16" s="251"/>
       <c r="C16" s="303" t="s">
@@ -14333,7 +14690,7 @@
       <c r="J16" s="82"/>
       <c r="K16" s="82"/>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" ht="17">
       <c r="A17" s="82"/>
       <c r="B17" s="251"/>
       <c r="C17" s="303" t="s">
@@ -14354,7 +14711,7 @@
       <c r="J17" s="82"/>
       <c r="K17" s="82"/>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" ht="17">
       <c r="A18" s="82"/>
       <c r="B18" s="251"/>
       <c r="C18" s="303" t="s">
@@ -14388,7 +14745,7 @@
       <c r="J19" s="82"/>
       <c r="K19" s="82"/>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" ht="17">
       <c r="A20" s="82"/>
       <c r="B20" s="304" t="s">
         <v>51</v>
@@ -14403,7 +14760,7 @@
       <c r="J20" s="82"/>
       <c r="K20" s="82"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" ht="17">
       <c r="A21" s="82"/>
       <c r="B21" s="251"/>
       <c r="C21" s="303" t="s">
@@ -14424,7 +14781,7 @@
       <c r="J21" s="82"/>
       <c r="K21" s="82"/>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" ht="17">
       <c r="A22" s="82"/>
       <c r="B22" s="251"/>
       <c r="C22" s="303" t="s">
@@ -14445,7 +14802,7 @@
       <c r="J22" s="82"/>
       <c r="K22" s="82"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" ht="17">
       <c r="A23" s="82"/>
       <c r="B23" s="251"/>
       <c r="C23" s="303" t="s">
@@ -14479,7 +14836,7 @@
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" ht="17">
       <c r="A25" s="82"/>
       <c r="B25" s="304" t="s">
         <v>192</v>
@@ -14494,7 +14851,7 @@
       <c r="J25" s="82"/>
       <c r="K25" s="82"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" ht="17">
       <c r="A26" s="82"/>
       <c r="B26" s="251"/>
       <c r="C26" s="303" t="s">
@@ -14515,7 +14872,7 @@
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" ht="17">
       <c r="A27" s="82"/>
       <c r="B27" s="251"/>
       <c r="C27" s="303" t="s">
@@ -14536,7 +14893,7 @@
       <c r="J27" s="82"/>
       <c r="K27" s="82"/>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" ht="17">
       <c r="A28" s="82"/>
       <c r="B28" s="251"/>
       <c r="C28" s="303" t="s">
@@ -15018,8 +15375,8 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet14" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr codeName="Sheet14">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B2:M26"/>
@@ -15028,14 +15385,14 @@
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="82"/>
-    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
-    <col min="5" max="13" width="15.875" style="82" customWidth="1"/>
-    <col min="14" max="16384" width="10.625" style="82"/>
+    <col min="1" max="1" width="10.6640625" style="82"/>
+    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
+    <col min="5" max="13" width="15.83203125" style="82" customWidth="1"/>
+    <col min="14" max="16384" width="10.6640625" style="82"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21">
@@ -15070,14 +15427,14 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:13" ht="107" customHeight="1">
-      <c r="B5" s="361" t="s">
+      <c r="B5" s="363" t="s">
         <v>405</v>
       </c>
-      <c r="C5" s="362"/>
-      <c r="D5" s="362"/>
-      <c r="E5" s="362"/>
-      <c r="F5" s="362"/>
-      <c r="G5" s="363"/>
+      <c r="C5" s="364"/>
+      <c r="D5" s="364"/>
+      <c r="E5" s="364"/>
+      <c r="F5" s="364"/>
+      <c r="G5" s="365"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:13" ht="17" thickBot="1"/>
@@ -15111,7 +15468,7 @@
       <c r="L8" s="110"/>
       <c r="M8" s="111"/>
     </row>
-    <row r="9" spans="2:13">
+    <row r="9" spans="2:13" ht="17">
       <c r="B9" s="132" t="s">
         <v>261</v>
       </c>
@@ -15161,7 +15518,7 @@
       <c r="L10" s="113"/>
       <c r="M10" s="130"/>
     </row>
-    <row r="11" spans="2:13">
+    <row r="11" spans="2:13" ht="17">
       <c r="B11" s="134"/>
       <c r="C11" s="246" t="s">
         <v>126</v>
@@ -15217,7 +15574,7 @@
       <c r="L12" s="217"/>
       <c r="M12" s="218"/>
     </row>
-    <row r="13" spans="2:13">
+    <row r="13" spans="2:13" ht="34">
       <c r="B13" s="135" t="s">
         <v>277</v>
       </c>
@@ -15233,7 +15590,7 @@
       <c r="L13" s="167"/>
       <c r="M13" s="168"/>
     </row>
-    <row r="14" spans="2:13">
+    <row r="14" spans="2:13" ht="17">
       <c r="B14" s="134"/>
       <c r="C14" s="246" t="s">
         <v>25</v>
@@ -15275,7 +15632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:13">
+    <row r="15" spans="2:13" ht="17">
       <c r="B15" s="136"/>
       <c r="C15" s="247" t="s">
         <v>142</v>
@@ -15317,7 +15674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13">
+    <row r="16" spans="2:13" ht="17">
       <c r="B16" s="136"/>
       <c r="C16" s="247" t="s">
         <v>309</v>
@@ -15359,7 +15716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" ht="17">
       <c r="B17" s="136"/>
       <c r="C17" s="247" t="s">
         <v>310</v>
@@ -15399,7 +15756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" ht="17">
       <c r="B18" s="136"/>
       <c r="C18" s="247" t="s">
         <v>82</v>
@@ -15455,7 +15812,7 @@
       <c r="L19" s="217"/>
       <c r="M19" s="218"/>
     </row>
-    <row r="20" spans="2:13" ht="32">
+    <row r="20" spans="2:13" ht="34">
       <c r="B20" s="135" t="s">
         <v>278</v>
       </c>
@@ -15471,7 +15828,7 @@
       <c r="L20" s="167"/>
       <c r="M20" s="168"/>
     </row>
-    <row r="21" spans="2:13">
+    <row r="21" spans="2:13" ht="17">
       <c r="B21" s="134"/>
       <c r="C21" s="246" t="s">
         <v>216</v>
@@ -15513,7 +15870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
+    <row r="22" spans="2:13" ht="17">
       <c r="B22" s="134"/>
       <c r="C22" s="248" t="s">
         <v>275</v>
@@ -15555,7 +15912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
+    <row r="23" spans="2:13" ht="17">
       <c r="B23" s="134"/>
       <c r="C23" s="248" t="s">
         <v>309</v>
@@ -15589,7 +15946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
+    <row r="24" spans="2:13" ht="17">
       <c r="B24" s="134"/>
       <c r="C24" s="248" t="s">
         <v>310</v>
@@ -15626,7 +15983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
+    <row r="25" spans="2:13" ht="17">
       <c r="B25" s="134"/>
       <c r="C25" s="248" t="s">
         <v>82</v>
@@ -15702,8 +16059,8 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet13" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr codeName="Sheet13">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B2:L12"/>
@@ -15712,14 +16069,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="82"/>
-    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
-    <col min="5" max="13" width="15.875" style="82" customWidth="1"/>
-    <col min="14" max="16384" width="10.625" style="82"/>
+    <col min="1" max="1" width="10.6640625" style="82"/>
+    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
+    <col min="5" max="13" width="15.83203125" style="82" customWidth="1"/>
+    <col min="14" max="16384" width="10.6640625" style="82"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="21">
@@ -15757,15 +16114,15 @@
       <c r="I4" s="8"/>
     </row>
     <row r="5" spans="2:12" ht="26" customHeight="1">
-      <c r="B5" s="361" t="s">
+      <c r="B5" s="363" t="s">
         <v>449</v>
       </c>
-      <c r="C5" s="362"/>
-      <c r="D5" s="362"/>
-      <c r="E5" s="362"/>
-      <c r="F5" s="362"/>
-      <c r="G5" s="362"/>
-      <c r="H5" s="363"/>
+      <c r="C5" s="364"/>
+      <c r="D5" s="364"/>
+      <c r="E5" s="364"/>
+      <c r="F5" s="364"/>
+      <c r="G5" s="364"/>
+      <c r="H5" s="365"/>
       <c r="I5" s="8"/>
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1"/>
@@ -15801,7 +16158,7 @@
       <c r="K8" s="110"/>
       <c r="L8" s="111"/>
     </row>
-    <row r="9" spans="2:12" ht="32">
+    <row r="9" spans="2:12" ht="34">
       <c r="B9" s="132" t="s">
         <v>261</v>
       </c>
@@ -15847,7 +16204,7 @@
       <c r="K10" s="113"/>
       <c r="L10" s="130"/>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:12" ht="17">
       <c r="B11" s="134"/>
       <c r="C11" s="246" t="s">
         <v>309</v>
@@ -15919,8 +16276,8 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet27" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr codeName="Sheet27">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B2:I16"/>
@@ -15929,14 +16286,14 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="82"/>
-    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
-    <col min="5" max="10" width="15.875" style="82" customWidth="1"/>
-    <col min="11" max="16384" width="10.625" style="82"/>
+    <col min="1" max="1" width="10.6640625" style="82"/>
+    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
+    <col min="5" max="10" width="15.83203125" style="82" customWidth="1"/>
+    <col min="11" max="16384" width="10.6640625" style="82"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="21">
@@ -15968,13 +16325,13 @@
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="2:9" ht="37" customHeight="1">
-      <c r="B5" s="361" t="s">
+      <c r="B5" s="363" t="s">
         <v>447</v>
       </c>
-      <c r="C5" s="362"/>
-      <c r="D5" s="362"/>
-      <c r="E5" s="362"/>
-      <c r="F5" s="363"/>
+      <c r="C5" s="364"/>
+      <c r="D5" s="364"/>
+      <c r="E5" s="364"/>
+      <c r="F5" s="365"/>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="2:9" ht="17" thickBot="1"/>
@@ -16000,7 +16357,7 @@
       <c r="H8" s="110"/>
       <c r="I8" s="111"/>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" ht="17">
       <c r="B9" s="132"/>
       <c r="C9" s="219"/>
       <c r="D9" s="141"/>
@@ -16032,7 +16389,7 @@
       <c r="H10" s="113"/>
       <c r="I10" s="130"/>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" ht="17">
       <c r="B11" s="134"/>
       <c r="C11" s="246" t="s">
         <v>309</v>
@@ -16079,7 +16436,7 @@
       <c r="H13" s="321"/>
       <c r="I13" s="322"/>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" ht="17">
       <c r="B14" s="135" t="s">
         <v>445</v>
       </c>
@@ -16091,7 +16448,7 @@
       <c r="H14" s="167"/>
       <c r="I14" s="168"/>
     </row>
-    <row r="15" spans="2:9">
+    <row r="15" spans="2:9" ht="17">
       <c r="B15" s="134"/>
       <c r="C15" s="246" t="s">
         <v>309</v>
@@ -16148,24 +16505,24 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet28" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr codeName="Sheet28">
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="82"/>
-    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
-    <col min="5" max="11" width="15.875" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="82"/>
+    <col min="1" max="1" width="10.6640625" style="82"/>
+    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
+    <col min="5" max="11" width="15.83203125" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="82"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21">
@@ -16200,14 +16557,14 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="84" customHeight="1">
-      <c r="B5" s="361" t="s">
+      <c r="B5" s="363" t="s">
         <v>451</v>
       </c>
-      <c r="C5" s="362"/>
-      <c r="D5" s="362"/>
-      <c r="E5" s="362"/>
-      <c r="F5" s="362"/>
-      <c r="G5" s="363"/>
+      <c r="C5" s="364"/>
+      <c r="D5" s="364"/>
+      <c r="E5" s="364"/>
+      <c r="F5" s="364"/>
+      <c r="G5" s="365"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:8" ht="17" thickBot="1"/>
@@ -16227,7 +16584,7 @@
       <c r="E8" s="110"/>
       <c r="F8" s="111"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" ht="17">
       <c r="B9" s="132" t="s">
         <v>429</v>
       </c>
@@ -16240,7 +16597,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="17">
       <c r="B10" s="135" t="s">
         <v>430</v>
       </c>
@@ -16249,7 +16606,7 @@
       <c r="E10" s="167"/>
       <c r="F10" s="168"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" ht="17">
       <c r="B11" s="135"/>
       <c r="C11" s="246" t="s">
         <v>51</v>
@@ -16260,71 +16617,70 @@
         <v>0</v>
       </c>
       <c r="F11" s="324">
-        <f>IF(SUM($E$11:$E$12)=0,1,E11/SUM($E$11:$E$12))</f>
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="135"/>
-      <c r="C12" s="246" t="s">
-        <v>431</v>
-      </c>
-      <c r="D12" s="143"/>
-      <c r="E12" s="167">
-        <f>SUMIF('Refineries heat production'!E15:I15,"&gt;0")</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="324">
-        <f>IF(SUM($E$11:$E$12)=0,0,E12/SUM($E$11:$E$12))</f>
-        <v>0</v>
-      </c>
+      <c r="B12" s="323"/>
+      <c r="C12" s="221"/>
+      <c r="D12" s="216"/>
+      <c r="E12" s="217"/>
+      <c r="F12" s="218"/>
     </row>
     <row r="13" spans="2:8">
-      <c r="B13" s="323"/>
-      <c r="C13" s="221"/>
-      <c r="D13" s="216"/>
-      <c r="E13" s="217"/>
-      <c r="F13" s="218"/>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="135"/>
+      <c r="B13" s="135"/>
+      <c r="C13" s="246"/>
+      <c r="D13" s="143"/>
+      <c r="E13" s="167"/>
+      <c r="F13" s="168"/>
+    </row>
+    <row r="14" spans="2:8" ht="17">
+      <c r="B14" s="135" t="s">
+        <v>432</v>
+      </c>
       <c r="C14" s="246"/>
       <c r="D14" s="143"/>
       <c r="E14" s="167"/>
       <c r="F14" s="168"/>
     </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="135" t="s">
-        <v>432</v>
-      </c>
-      <c r="C15" s="246"/>
+    <row r="15" spans="2:8" ht="17">
+      <c r="B15" s="135"/>
+      <c r="C15" s="246" t="s">
+        <v>56</v>
+      </c>
       <c r="D15" s="143"/>
-      <c r="E15" s="167"/>
-      <c r="F15" s="168"/>
-    </row>
-    <row r="16" spans="2:8">
-      <c r="B16" s="135"/>
+      <c r="E15" s="167">
+        <f>'Refineries transformation'!F11</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="334">
+        <f t="shared" ref="F15:F21" si="0">IF(SUM($E$15:$E$22)=0,0,E15/SUM($E$15:$E$22))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="17">
+      <c r="B16" s="134"/>
       <c r="C16" s="246" t="s">
-        <v>56</v>
+        <v>433</v>
       </c>
       <c r="D16" s="143"/>
       <c r="E16" s="167">
-        <f>'Refineries transformation'!F11</f>
+        <f>'Refineries transformation'!G11</f>
         <v>0</v>
       </c>
       <c r="F16" s="334">
-        <f t="shared" ref="F16:F22" si="0">IF(SUM($E$16:$E$23)=0,0,E16/SUM($E$16:$E$23))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" ht="17">
       <c r="B17" s="134"/>
       <c r="C17" s="246" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D17" s="143"/>
       <c r="E17" s="167">
-        <f>'Refineries transformation'!G11</f>
+        <f>'Refineries transformation'!H11</f>
         <v>0</v>
       </c>
       <c r="F17" s="334">
@@ -16332,14 +16688,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="17">
       <c r="B18" s="134"/>
       <c r="C18" s="246" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="D18" s="143"/>
       <c r="E18" s="167">
-        <f>'Refineries transformation'!H11</f>
+        <f>'Refineries transformation'!I11</f>
         <v>0</v>
       </c>
       <c r="F18" s="334">
@@ -16347,14 +16703,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" ht="17">
       <c r="B19" s="134"/>
       <c r="C19" s="246" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D19" s="143"/>
       <c r="E19" s="167">
-        <f>'Refineries transformation'!I11</f>
+        <f>'Refineries transformation'!J11</f>
         <v>0</v>
       </c>
       <c r="F19" s="334">
@@ -16362,14 +16718,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" ht="17">
       <c r="B20" s="134"/>
       <c r="C20" s="246" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D20" s="143"/>
       <c r="E20" s="167">
-        <f>'Refineries transformation'!J11</f>
+        <f>'Refineries transformation'!K11</f>
         <v>0</v>
       </c>
       <c r="F20" s="334">
@@ -16377,14 +16733,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" ht="17">
       <c r="B21" s="134"/>
       <c r="C21" s="246" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D21" s="143"/>
       <c r="E21" s="167">
-        <f>'Refineries transformation'!K11</f>
+        <f>'Refineries transformation'!L11</f>
         <v>0</v>
       </c>
       <c r="F21" s="334">
@@ -16392,53 +16748,38 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" ht="17">
       <c r="B22" s="134"/>
-      <c r="C22" s="246" t="s">
-        <v>438</v>
+      <c r="C22" s="326" t="s">
+        <v>441</v>
       </c>
       <c r="D22" s="143"/>
       <c r="E22" s="167">
-        <f>'Refineries transformation'!L11</f>
+        <f>E11-SUM(E15:E21)</f>
         <v>0</v>
       </c>
       <c r="F22" s="334">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6">
-      <c r="B23" s="134"/>
-      <c r="C23" s="326" t="s">
-        <v>441</v>
-      </c>
-      <c r="D23" s="143"/>
-      <c r="E23" s="167">
-        <f>E12+E11-SUM(E16:E22)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="334">
-        <f>IF(SUM($E$16:$E$23)=0,1,E23/SUM($E$16:$E$23))</f>
+        <f>IF(SUM($E$15:$E$22)=0,1,E22/SUM($E$15:$E$22))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="17" thickBot="1">
-      <c r="B24" s="137"/>
-      <c r="C24" s="223"/>
-      <c r="D24" s="146"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="99"/>
+    <row r="23" spans="2:6" ht="17" thickBot="1">
+      <c r="B23" s="137"/>
+      <c r="C23" s="223"/>
+      <c r="D23" s="146"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="99"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="F24">
+  <conditionalFormatting sqref="F23">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E24">
+  <conditionalFormatting sqref="E23">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -16454,8 +16795,8 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
     <tabColor theme="5" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:H21"/>
@@ -16464,14 +16805,14 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="82"/>
-    <col min="2" max="2" width="25.875" style="82" customWidth="1"/>
-    <col min="3" max="3" width="30.875" style="82" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="82" customWidth="1"/>
-    <col min="5" max="11" width="15.875" style="82" customWidth="1"/>
-    <col min="12" max="16384" width="10.625" style="82"/>
+    <col min="1" max="1" width="10.6640625" style="82"/>
+    <col min="2" max="2" width="25.83203125" style="82" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="82" customWidth="1"/>
+    <col min="4" max="4" width="2.83203125" style="82" customWidth="1"/>
+    <col min="5" max="11" width="15.83203125" style="82" customWidth="1"/>
+    <col min="12" max="16384" width="10.6640625" style="82"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="21">
@@ -16506,14 +16847,14 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="24" customHeight="1">
-      <c r="B5" s="361" t="s">
+      <c r="B5" s="363" t="s">
         <v>454</v>
       </c>
-      <c r="C5" s="362"/>
-      <c r="D5" s="362"/>
-      <c r="E5" s="362"/>
-      <c r="F5" s="362"/>
-      <c r="G5" s="363"/>
+      <c r="C5" s="364"/>
+      <c r="D5" s="364"/>
+      <c r="E5" s="364"/>
+      <c r="F5" s="364"/>
+      <c r="G5" s="365"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:8" ht="17" thickBot="1"/>
@@ -16533,7 +16874,7 @@
       <c r="E8" s="110"/>
       <c r="F8" s="111"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" ht="17">
       <c r="B9" s="132" t="s">
         <v>429</v>
       </c>
@@ -16546,7 +16887,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" ht="17">
       <c r="B10" s="135" t="s">
         <v>445</v>
       </c>
@@ -16555,7 +16896,7 @@
       <c r="E10" s="167"/>
       <c r="F10" s="168"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" ht="17">
       <c r="B11" s="135"/>
       <c r="C11" s="246" t="s">
         <v>190</v>
@@ -16567,7 +16908,7 @@
       </c>
       <c r="F11" s="334"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" ht="17">
       <c r="B12" s="134"/>
       <c r="C12" s="246" t="s">
         <v>209</v>
@@ -16579,7 +16920,7 @@
       </c>
       <c r="F12" s="334"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" ht="17">
       <c r="B13" s="134"/>
       <c r="C13" s="246" t="s">
         <v>51</v>
@@ -16591,7 +16932,7 @@
       </c>
       <c r="F13" s="334"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" ht="17">
       <c r="B14" s="134"/>
       <c r="C14" s="246" t="s">
         <v>192</v>
@@ -16603,7 +16944,7 @@
       </c>
       <c r="F14" s="334"/>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" ht="17">
       <c r="B15" s="134"/>
       <c r="C15" s="246" t="s">
         <v>104</v>
@@ -16629,7 +16970,7 @@
       <c r="E17" s="321"/>
       <c r="F17" s="336"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" ht="17">
       <c r="B18" s="135" t="s">
         <v>430</v>
       </c>
@@ -16638,7 +16979,7 @@
       <c r="E18" s="167"/>
       <c r="F18" s="168"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" ht="17">
       <c r="B19" s="135"/>
       <c r="C19" s="246" t="s">
         <v>452</v>
@@ -16653,7 +16994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" ht="17">
       <c r="B20" s="135"/>
       <c r="C20" s="246" t="s">
         <v>431</v>
@@ -16700,8 +17041,8 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr codeName="Sheet15">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J6"/>
@@ -16710,10 +17051,10 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -16876,8 +17217,8 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet16" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr codeName="Sheet16">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -16886,10 +17227,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17020,8 +17361,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Sheet2">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:D16"/>
@@ -17030,13 +17371,13 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="20.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="90" customWidth="1"/>
-    <col min="5" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="50.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="90" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" ht="21">
@@ -17071,7 +17412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" ht="34">
       <c r="B7" s="77">
         <v>41611</v>
       </c>
@@ -17104,7 +17445,7 @@
         <v>1.03</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="32">
+    <row r="10" spans="2:4" ht="34">
       <c r="B10" s="120">
         <v>42576</v>
       </c>
@@ -17115,7 +17456,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" ht="34">
       <c r="B11" s="120">
         <v>42594</v>
       </c>
@@ -17126,7 +17467,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" ht="17">
       <c r="B12" s="120">
         <v>42615</v>
       </c>
@@ -17162,8 +17503,8 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet17" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr codeName="Sheet17">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -17172,10 +17513,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17306,8 +17647,8 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet18" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr codeName="Sheet18">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -17316,10 +17657,10 @@
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17450,8 +17791,8 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet19" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+  <sheetPr codeName="Sheet19">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -17460,10 +17801,10 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17594,8 +17935,8 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet20" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr codeName="Sheet20">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -17604,10 +17945,10 @@
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17738,8 +18079,8 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:B6"/>
@@ -17748,9 +18089,9 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="52.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -17813,8 +18154,8 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet21" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+  <sheetPr codeName="Sheet21">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -17823,12 +18164,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="52.5" style="277" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.5" style="277" bestFit="1" customWidth="1"/>
-    <col min="3" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -17959,8 +18300,8 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet22" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+  <sheetPr codeName="Sheet22">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -17969,10 +18310,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18103,8 +18444,8 @@
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet23" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+  <sheetPr codeName="Sheet23">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -18113,10 +18454,10 @@
       <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18247,8 +18588,8 @@
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet24" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+  <sheetPr codeName="Sheet24">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -18257,11 +18598,11 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="54" style="277" customWidth="1"/>
-    <col min="2" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18385,8 +18726,8 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet25" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+  <sheetPr codeName="Sheet25">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J10"/>
@@ -18395,10 +18736,10 @@
       <selection activeCell="C16" sqref="C16:G36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18529,8 +18870,8 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet3" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Sheet3">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:C34"/>
@@ -18539,12 +18880,12 @@
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="35.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="100.875" style="116" customWidth="1"/>
-    <col min="4" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="35.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="100.83203125" style="116" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="21">
@@ -18812,21 +19153,21 @@
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet26" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+  <sheetPr codeName="Sheet26">
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27" style="277" customWidth="1"/>
-    <col min="2" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -18853,33 +19194,41 @@
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="278" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="B4" s="317">
-        <f>'Refineries efficiency'!F12</f>
+        <f>'Refineries efficiency'!F15</f>
         <v>0</v>
       </c>
+      <c r="C4" s="296"/>
+      <c r="D4" s="193"/>
+      <c r="E4" s="193"/>
+      <c r="F4" s="193"/>
+      <c r="G4" s="193"/>
+      <c r="H4" s="193"/>
+      <c r="I4" s="193"/>
+      <c r="J4" s="193"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="278" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B5" s="317">
         <f>'Refineries efficiency'!F16</f>
         <v>0</v>
       </c>
       <c r="C5" s="296"/>
-      <c r="D5" s="193"/>
-      <c r="E5" s="193"/>
-      <c r="F5" s="193"/>
-      <c r="G5" s="193"/>
-      <c r="H5" s="193"/>
-      <c r="I5" s="193"/>
-      <c r="J5" s="193"/>
+      <c r="D5" s="296"/>
+      <c r="E5" s="296"/>
+      <c r="F5" s="296"/>
+      <c r="G5" s="296"/>
+      <c r="H5" s="296"/>
+      <c r="I5" s="296"/>
+      <c r="J5" s="296"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="278" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B6" s="317">
         <f>'Refineries efficiency'!F17</f>
@@ -18896,30 +19245,30 @@
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="278" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B7" s="317">
         <f>'Refineries efficiency'!F18</f>
         <v>0</v>
       </c>
-      <c r="C7" s="296"/>
-      <c r="D7" s="296"/>
-      <c r="E7" s="296"/>
-      <c r="F7" s="296"/>
-      <c r="G7" s="296"/>
-      <c r="H7" s="296"/>
-      <c r="I7" s="296"/>
-      <c r="J7" s="296"/>
+      <c r="C7" s="193"/>
+      <c r="D7" s="193"/>
+      <c r="E7" s="193"/>
+      <c r="F7" s="193"/>
+      <c r="G7" s="193"/>
+      <c r="H7" s="193"/>
+      <c r="I7" s="193"/>
+      <c r="J7" s="193"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="278" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B8" s="317">
         <f>'Refineries efficiency'!F19</f>
         <v>0</v>
       </c>
-      <c r="C8" s="193"/>
+      <c r="C8" s="296"/>
       <c r="D8" s="193"/>
       <c r="E8" s="193"/>
       <c r="F8" s="193"/>
@@ -18930,14 +19279,14 @@
     </row>
     <row r="9" spans="1:10">
       <c r="A9" s="278" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="B9" s="317">
         <f>'Refineries efficiency'!F20</f>
         <v>0</v>
       </c>
       <c r="C9" s="296"/>
-      <c r="D9" s="193"/>
+      <c r="D9" s="301"/>
       <c r="E9" s="193"/>
       <c r="F9" s="193"/>
       <c r="G9" s="193"/>
@@ -18947,27 +19296,10 @@
     </row>
     <row r="10" spans="1:10">
       <c r="A10" s="278" t="s">
-        <v>426</v>
+        <v>463</v>
       </c>
       <c r="B10" s="317">
         <f>'Refineries efficiency'!F21</f>
-        <v>0</v>
-      </c>
-      <c r="C10" s="296"/>
-      <c r="D10" s="301"/>
-      <c r="E10" s="193"/>
-      <c r="F10" s="193"/>
-      <c r="G10" s="193"/>
-      <c r="H10" s="193"/>
-      <c r="I10" s="193"/>
-      <c r="J10" s="193"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="278" t="s">
-        <v>463</v>
-      </c>
-      <c r="B11" s="317">
-        <f>'Refineries efficiency'!F22</f>
         <v>0</v>
       </c>
     </row>
@@ -18983,8 +19315,8 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+  <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="A1:J11"/>
@@ -18993,11 +19325,11 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27" style="277" customWidth="1"/>
-    <col min="2" max="10" width="11.625" style="277" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="11.6640625" style="277" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -19118,19 +19450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:B20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="140.875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="140.83203125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="21">
@@ -19146,7 +19478,7 @@
     <row r="5" spans="2:2">
       <c r="B5" s="42"/>
     </row>
-    <row r="6" spans="2:2" ht="64">
+    <row r="6" spans="2:2" ht="68">
       <c r="B6" s="267" t="s">
         <v>305</v>
       </c>
@@ -19196,7 +19528,7 @@
     <row r="18" spans="2:2">
       <c r="B18" s="42"/>
     </row>
-    <row r="19" spans="2:2" ht="80">
+    <row r="19" spans="2:2" ht="102">
       <c r="B19" s="124" t="s">
         <v>247</v>
       </c>
@@ -19216,8 +19548,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet5" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Sheet5">
     <tabColor theme="2"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -19227,9 +19559,9 @@
       <selection activeCell="CV35" sqref="CV35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.875" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="16384" width="2.875" style="1"/>
+    <col min="1" max="16384" width="2.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:80" ht="20" customHeight="1">
@@ -19598,7 +19930,7 @@
       <c r="BU6" s="52"/>
       <c r="BV6" s="52"/>
     </row>
-    <row r="7" spans="2:80" ht="25">
+    <row r="7" spans="2:80" ht="24">
       <c r="B7" s="52"/>
       <c r="C7" s="64" t="s">
         <v>182</v>
@@ -19693,8 +20025,8 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet6" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Sheet6">
     <tabColor theme="2"/>
   </sheetPr>
   <dimension ref="B2:C107"/>
@@ -19703,12 +20035,12 @@
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="25.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.875" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="25.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.83203125" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" ht="21">
@@ -19724,10 +20056,10 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:3" ht="75" customHeight="1">
-      <c r="B5" s="350" t="s">
+      <c r="B5" s="352" t="s">
         <v>248</v>
       </c>
-      <c r="C5" s="351"/>
+      <c r="C5" s="353"/>
     </row>
     <row r="6" spans="2:3" ht="17" thickBot="1"/>
     <row r="7" spans="2:3">
@@ -19754,31 +20086,31 @@
       </c>
       <c r="C10" s="27"/>
     </row>
-    <row r="11" spans="2:3" ht="32">
+    <row r="11" spans="2:3" ht="34">
       <c r="B11" s="22"/>
       <c r="C11" s="266" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="32">
+    <row r="12" spans="2:3" ht="34">
       <c r="B12" s="22"/>
       <c r="C12" s="266" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" ht="17">
       <c r="B13" s="22"/>
       <c r="C13" s="266" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="32">
+    <row r="14" spans="2:3" ht="34">
       <c r="B14" s="22"/>
       <c r="C14" s="266" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" ht="34">
       <c r="B15" s="22"/>
       <c r="C15" s="266" t="s">
         <v>227</v>
@@ -20262,7 +20594,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" ht="17">
       <c r="B98" s="22"/>
       <c r="C98" s="29" t="s">
         <v>26</v>
@@ -20326,34 +20658,32 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet7" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Sheet7">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A2:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
-    </sheetView>
+    <sheetView zoomScale="106" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="18.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="77.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="4.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="2.875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="45.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="4.375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="79.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="65.875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="2.875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="13.375" style="204" customWidth="1"/>
-    <col min="17" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="18.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="77.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="4.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="45.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="4.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="79.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="9.1640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="65.83203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="2.83203125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="13.33203125" style="204" customWidth="1"/>
+    <col min="17" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:16" ht="21">
@@ -20385,32 +20715,32 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:16">
-      <c r="B5" s="352" t="s">
+      <c r="B5" s="354" t="s">
         <v>307</v>
       </c>
-      <c r="C5" s="353"/>
-      <c r="D5" s="353"/>
-      <c r="E5" s="354"/>
+      <c r="C5" s="355"/>
+      <c r="D5" s="355"/>
+      <c r="E5" s="356"/>
       <c r="F5" s="8"/>
       <c r="I5" s="229"/>
       <c r="J5" s="8"/>
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:16">
-      <c r="B6" s="352"/>
-      <c r="C6" s="353"/>
-      <c r="D6" s="353"/>
-      <c r="E6" s="354"/>
+      <c r="B6" s="354"/>
+      <c r="C6" s="355"/>
+      <c r="D6" s="355"/>
+      <c r="E6" s="356"/>
       <c r="F6" s="8"/>
       <c r="I6" s="207"/>
       <c r="J6" s="8"/>
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="B7" s="350"/>
-      <c r="C7" s="355"/>
-      <c r="D7" s="355"/>
-      <c r="E7" s="351"/>
+      <c r="B7" s="352"/>
+      <c r="C7" s="357"/>
+      <c r="D7" s="357"/>
+      <c r="E7" s="353"/>
       <c r="F7" s="151"/>
       <c r="I7" s="228"/>
       <c r="J7" s="9"/>
@@ -20517,7 +20847,9 @@
         <v>205</v>
       </c>
       <c r="D13" s="157"/>
-      <c r="E13" s="162"/>
+      <c r="E13" s="162" t="s">
+        <v>479</v>
+      </c>
       <c r="F13" s="162"/>
       <c r="G13" s="15" t="s">
         <v>259</v>
@@ -20548,7 +20880,9 @@
         <v>258</v>
       </c>
       <c r="D14" s="157"/>
-      <c r="E14" s="162"/>
+      <c r="E14" s="162">
+        <v>2015</v>
+      </c>
       <c r="F14" s="162"/>
       <c r="G14" s="15" t="s">
         <v>260</v>
@@ -20613,7 +20947,7 @@
       <c r="O16" s="207"/>
       <c r="P16" s="208"/>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" ht="17">
       <c r="A17" s="8"/>
       <c r="B17" s="28"/>
       <c r="C17" s="258" t="s">
@@ -20638,7 +20972,7 @@
       <c r="O17" s="207"/>
       <c r="P17" s="208"/>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" ht="17">
       <c r="A18" s="8"/>
       <c r="B18" s="22"/>
       <c r="C18" s="258" t="s">
@@ -20671,7 +21005,7 @@
       <c r="O18" s="207"/>
       <c r="P18" s="208"/>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" ht="17">
       <c r="A19" s="8"/>
       <c r="B19" s="22"/>
       <c r="C19" s="258" t="s">
@@ -20696,7 +21030,7 @@
       <c r="O19" s="207"/>
       <c r="P19" s="208"/>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" ht="17">
       <c r="A20" s="8"/>
       <c r="B20" s="22"/>
       <c r="C20" s="258" t="s">
@@ -20721,7 +21055,7 @@
       <c r="O20" s="207"/>
       <c r="P20" s="208"/>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" ht="17">
       <c r="A21" s="8"/>
       <c r="B21" s="22"/>
       <c r="C21" s="258" t="s">
@@ -20746,7 +21080,7 @@
       <c r="O21" s="207"/>
       <c r="P21" s="208"/>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" ht="17">
       <c r="A22" s="8"/>
       <c r="B22" s="22"/>
       <c r="C22" s="258" t="s">
@@ -20771,7 +21105,7 @@
       <c r="O22" s="207"/>
       <c r="P22" s="208"/>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" ht="17">
       <c r="A23" s="8"/>
       <c r="B23" s="22"/>
       <c r="C23" s="258" t="s">
@@ -20796,7 +21130,7 @@
       <c r="O23" s="207"/>
       <c r="P23" s="208"/>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" ht="17">
       <c r="A24" s="8"/>
       <c r="B24" s="22"/>
       <c r="C24" s="258" t="s">
@@ -20867,7 +21201,7 @@
       <c r="O26" s="207"/>
       <c r="P26" s="208"/>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" ht="17">
       <c r="A27" s="8"/>
       <c r="B27" s="28"/>
       <c r="C27" s="258" t="s">
@@ -20892,7 +21226,7 @@
       <c r="O27" s="207"/>
       <c r="P27" s="208"/>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" ht="17">
       <c r="A28" s="8"/>
       <c r="B28" s="22"/>
       <c r="C28" s="258" t="s">
@@ -20925,7 +21259,7 @@
       <c r="O28" s="207"/>
       <c r="P28" s="208"/>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" ht="17">
       <c r="A29" s="8"/>
       <c r="B29" s="22"/>
       <c r="C29" s="258" t="s">
@@ -20950,7 +21284,7 @@
       <c r="O29" s="207"/>
       <c r="P29" s="208"/>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" ht="17">
       <c r="A30" s="8"/>
       <c r="B30" s="22"/>
       <c r="C30" s="258" t="s">
@@ -20975,7 +21309,7 @@
       <c r="O30" s="207"/>
       <c r="P30" s="208"/>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" ht="17">
       <c r="A31" s="8"/>
       <c r="B31" s="22"/>
       <c r="C31" s="258" t="s">
@@ -21000,7 +21334,7 @@
       <c r="O31" s="207"/>
       <c r="P31" s="208"/>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" ht="17">
       <c r="A32" s="8"/>
       <c r="B32" s="22"/>
       <c r="C32" s="258" t="s">
@@ -21025,7 +21359,7 @@
       <c r="O32" s="207"/>
       <c r="P32" s="208"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" ht="17">
       <c r="A33" s="8"/>
       <c r="B33" s="22"/>
       <c r="C33" s="258" t="s">
@@ -21050,7 +21384,7 @@
       <c r="O33" s="207"/>
       <c r="P33" s="208"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" ht="17">
       <c r="A34" s="8"/>
       <c r="B34" s="22"/>
       <c r="C34" s="258" t="s">
@@ -21168,8 +21502,8 @@
         <v>476</v>
       </c>
       <c r="D39" s="158"/>
-      <c r="E39" s="365"/>
-      <c r="G39" s="364"/>
+      <c r="E39" s="351"/>
+      <c r="G39" s="350"/>
       <c r="J39" s="8"/>
       <c r="K39" s="345" t="s">
         <v>473</v>
@@ -21211,7 +21545,7 @@
         <v>477</v>
       </c>
       <c r="D41" s="158"/>
-      <c r="E41" s="365"/>
+      <c r="E41" s="351"/>
       <c r="F41" s="126"/>
       <c r="G41" s="202"/>
       <c r="H41" s="8"/>
@@ -21244,7 +21578,7 @@
         <v>478</v>
       </c>
       <c r="D42" s="158"/>
-      <c r="E42" s="365"/>
+      <c r="E42" s="351"/>
       <c r="F42" s="126"/>
       <c r="G42" s="202"/>
       <c r="H42" s="8"/>
@@ -21277,7 +21611,7 @@
         <v>475</v>
       </c>
       <c r="D43" s="158"/>
-      <c r="E43" s="365"/>
+      <c r="E43" s="351"/>
       <c r="F43" s="126"/>
       <c r="G43" s="202"/>
       <c r="H43" s="8"/>
@@ -21430,7 +21764,7 @@
       <c r="O50" s="207"/>
       <c r="P50" s="208"/>
     </row>
-    <row r="51" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="51" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A51" s="8"/>
       <c r="B51" s="22"/>
       <c r="C51" s="258" t="s">
@@ -21462,7 +21796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="52" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A52" s="8"/>
       <c r="B52" s="22"/>
       <c r="C52" s="258" t="s">
@@ -21494,7 +21828,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="53" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A53" s="8"/>
       <c r="B53" s="22"/>
       <c r="C53" s="258" t="s">
@@ -21526,7 +21860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="54" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A54" s="8"/>
       <c r="B54" s="22"/>
       <c r="C54" s="258" t="s">
@@ -21558,7 +21892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="55" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A55" s="8"/>
       <c r="B55" s="22"/>
       <c r="C55" s="258" t="s">
@@ -21590,7 +21924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="56" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A56" s="8"/>
       <c r="B56" s="22"/>
       <c r="C56" s="258" t="s">
@@ -21660,7 +21994,7 @@
       <c r="O58" s="207"/>
       <c r="P58" s="208"/>
     </row>
-    <row r="59" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="59" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A59" s="8"/>
       <c r="B59" s="22"/>
       <c r="C59" s="258" t="s">
@@ -21692,7 +22026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="60" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A60" s="8"/>
       <c r="B60" s="22"/>
       <c r="C60" s="258" t="s">
@@ -21724,7 +22058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="17" outlineLevel="1" thickBot="1">
+    <row r="61" spans="1:16" ht="18" outlineLevel="1" thickBot="1">
       <c r="A61" s="8"/>
       <c r="B61" s="22"/>
       <c r="C61" s="258" t="s">
@@ -21887,7 +22221,7 @@
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="11265" r:id="rId3" name="import_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!import_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[3]!import_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -21905,12 +22239,11 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="11266" r:id="rId4" name="export_data">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!export_data_button">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[3]!export_data_button">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>8</xdr:col>
@@ -21928,12 +22261,11 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
             <control shapeId="11272" r:id="rId5" name="select_dashboard">
-              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[2]!select_dashboard_values">
+              <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[3]!select_dashboard_values">
                 <anchor moveWithCells="1" sizeWithCells="1">
                   <from>
                     <xdr:col>9</xdr:col>
@@ -21951,11 +22283,9 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -21966,8 +22296,8 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr codeName="Sheet8">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B2:BO101"/>
@@ -21979,12 +22309,12 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="50.875" style="1" customWidth="1"/>
-    <col min="3" max="67" width="13.625" style="1" customWidth="1"/>
-    <col min="68" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="50.83203125" style="1" customWidth="1"/>
+    <col min="3" max="67" width="13.6640625" style="1" customWidth="1"/>
+    <col min="68" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:67" ht="21">
@@ -22000,7 +22330,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="32">
+    <row r="5" spans="2:67" ht="34">
       <c r="B5" s="125" t="s">
         <v>256</v>
       </c>
@@ -28799,24 +29129,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet9" enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr codeName="Sheet9">
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
   <dimension ref="B1:M18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="1"/>
-    <col min="2" max="2" width="21.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.125" style="1" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="52.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="19" width="14.125" style="1" customWidth="1"/>
-    <col min="20" max="21" width="20.875" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="10.625" style="1"/>
+    <col min="1" max="1" width="10.6640625" style="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="19" width="14.1640625" style="1" customWidth="1"/>
+    <col min="20" max="21" width="20.83203125" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="10.6640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
@@ -28849,11 +29179,11 @@
       <c r="M4" s="8"/>
     </row>
     <row r="5" spans="2:13" ht="60" customHeight="1">
-      <c r="B5" s="356" t="s">
+      <c r="B5" s="358" t="s">
         <v>300</v>
       </c>
-      <c r="C5" s="357"/>
-      <c r="D5" s="357"/>
+      <c r="C5" s="359"/>
+      <c r="D5" s="359"/>
       <c r="E5" s="272"/>
       <c r="F5" s="45"/>
       <c r="G5" s="45"/>
@@ -28902,7 +29232,7 @@
       </c>
       <c r="G9" s="23"/>
     </row>
-    <row r="10" spans="2:13">
+    <row r="10" spans="2:13" ht="17">
       <c r="B10" s="91" t="s">
         <v>280</v>
       </c>

</xml_diff>